<commit_message>
Dismiss all Misdemeanors and Infractions
[#166588943]

Co-authored-by: Zak Auerbach <zak@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="272">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>4.5</t>
+  </si>
+  <si>
+    <t>Misdemeanor or Infraction</t>
   </si>
   <si>
     <t>11359HS-INTENT SELL CANNABIS</t>
@@ -1063,8 +1066,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1304,7 +1319,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1322,6 +1337,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1339,6 +1356,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2499,8 +2518,8 @@
   </sheetPr>
   <dimension ref="B1:DD35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CV2" workbookViewId="0">
-      <selection activeCell="CY22" sqref="CY22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CD3" workbookViewId="0">
+      <selection activeCell="CF35" sqref="CF35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2606,7 +2625,7 @@
   <sheetData>
     <row r="1" spans="2:108" s="42" customFormat="1" ht="27.75" customHeight="1">
       <c r="B1" s="39" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
@@ -2619,16 +2638,16 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
       <c r="M1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="P1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q1" s="41"/>
       <c r="R1" s="41"/>
@@ -2638,7 +2657,7 @@
       <c r="V1" s="41"/>
       <c r="W1" s="41"/>
       <c r="X1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Y1" s="41"/>
       <c r="Z1" s="41"/>
@@ -2655,12 +2674,12 @@
       <c r="AK1" s="41"/>
       <c r="AL1" s="41"/>
       <c r="AM1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN1" s="41"/>
       <c r="AO1" s="41"/>
       <c r="AP1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AQ1" s="41"/>
       <c r="AR1" s="41"/>
@@ -2668,23 +2687,23 @@
       <c r="AT1" s="41"/>
       <c r="AU1" s="41"/>
       <c r="AV1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AW1" s="41"/>
       <c r="AX1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AY1" s="41"/>
       <c r="AZ1" s="41"/>
       <c r="BA1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="BB1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="BC1" s="41"/>
       <c r="BD1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="BE1" s="41"/>
       <c r="BF1" s="41"/>
@@ -2712,71 +2731,71 @@
       <c r="CB1" s="41"/>
       <c r="CC1" s="41"/>
       <c r="CD1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CE1" s="41"/>
       <c r="CF1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CG1" s="41"/>
       <c r="CH1" s="41"/>
       <c r="CI1" s="41"/>
       <c r="CJ1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CK1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CL1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CM1" s="41"/>
       <c r="CN1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CO1" s="41"/>
       <c r="CP1" s="41"/>
       <c r="CQ1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CR1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CS1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CT1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CU1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CV1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CW1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CX1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CY1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="CZ1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DA1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DB1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DC1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="DD1" s="41" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="2:108" ht="20.25" customHeight="1">
@@ -3236,7 +3255,7 @@
         <v>107</v>
       </c>
       <c r="AZ3" s="33" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="BA3" s="5">
         <v>19790525</v>
@@ -3453,7 +3472,7 @@
         <v>107</v>
       </c>
       <c r="AZ4" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="BA4" s="10">
         <v>19790601</v>
@@ -3680,7 +3699,7 @@
         <v>107</v>
       </c>
       <c r="AZ5" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="BA5" s="10">
         <v>19810410</v>
@@ -3897,7 +3916,7 @@
         <v>107</v>
       </c>
       <c r="AZ6" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="BA6" s="10">
         <v>19810410</v>
@@ -4114,7 +4133,7 @@
         <v>107</v>
       </c>
       <c r="AZ7" s="34" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="BA7" s="10">
         <v>19810411</v>
@@ -4331,7 +4350,7 @@
         <v>107</v>
       </c>
       <c r="AZ8" s="34" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="BA8" s="10">
         <v>19810411</v>
@@ -4445,7 +4464,7 @@
         <v>150</v>
       </c>
       <c r="DD8" s="11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="2:108" ht="20" customHeight="1">
@@ -4582,7 +4601,7 @@
         <v>107</v>
       </c>
       <c r="AZ9" s="37" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="BA9" s="25">
         <v>19790525</v>
@@ -4799,7 +4818,7 @@
         <v>107</v>
       </c>
       <c r="AZ10" s="37" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="BA10" s="25">
         <v>19790601</v>
@@ -4901,7 +4920,7 @@
         <v>159</v>
       </c>
       <c r="CZ10" s="26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="DA10" s="26" t="s">
         <v>145</v>
@@ -4913,7 +4932,7 @@
         <v>150</v>
       </c>
       <c r="DD10" s="26" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="2:108" ht="20" customHeight="1">
@@ -5050,7 +5069,7 @@
         <v>107</v>
       </c>
       <c r="AZ11" s="37" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="BA11" s="25">
         <v>19790601</v>
@@ -5263,7 +5282,7 @@
         <v>107</v>
       </c>
       <c r="AZ12" s="37" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="BA12" s="25">
         <v>19851101</v>
@@ -5275,7 +5294,7 @@
         <v>107</v>
       </c>
       <c r="BD12" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="BE12" s="26" t="s">
         <v>115</v>
@@ -5359,13 +5378,13 @@
         <v>157</v>
       </c>
       <c r="CX12" s="26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="CY12" s="26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="CZ12" s="26" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="DA12" s="26" t="s">
         <v>145</v>
@@ -5377,7 +5396,7 @@
         <v>185</v>
       </c>
       <c r="DD12" s="26" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="2:108" ht="20" customHeight="1">
@@ -5514,7 +5533,7 @@
         <v>107</v>
       </c>
       <c r="AZ13" s="37" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="BA13" s="25">
         <v>19851101</v>
@@ -5735,7 +5754,7 @@
         <v>107</v>
       </c>
       <c r="AZ14" s="35" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="BA14" s="15">
         <v>19810411</v>
@@ -5839,7 +5858,7 @@
         <v>148</v>
       </c>
       <c r="CZ14" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="DA14" s="16" t="s">
         <v>169</v>
@@ -5851,7 +5870,7 @@
         <v>150</v>
       </c>
       <c r="DD14" s="17" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="2:108" ht="20" hidden="1" customHeight="1">
@@ -5988,7 +6007,7 @@
         <v>173</v>
       </c>
       <c r="AZ15" s="35" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="BA15" s="15">
         <v>19810411</v>
@@ -6215,7 +6234,7 @@
         <v>173</v>
       </c>
       <c r="AZ16" s="35" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="BA16" s="15">
         <v>19810411</v>
@@ -6442,7 +6461,7 @@
         <v>107</v>
       </c>
       <c r="AZ17" s="35" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="BA17" s="15">
         <v>19810411</v>
@@ -6538,13 +6557,13 @@
         <v>146</v>
       </c>
       <c r="CX17" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="CY17" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="CY17" s="16" t="s">
-        <v>260</v>
-      </c>
       <c r="CZ17" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="DA17" s="16" t="s">
         <v>169</v>
@@ -6556,7 +6575,7 @@
         <v>185</v>
       </c>
       <c r="DD17" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="2:108" ht="20" customHeight="1">
@@ -6693,7 +6712,7 @@
         <v>107</v>
       </c>
       <c r="AZ18" s="35" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="BA18" s="15">
         <v>19810411</v>
@@ -6918,7 +6937,7 @@
         <v>107</v>
       </c>
       <c r="AZ19" s="36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="BA19" s="20">
         <v>19810411</v>
@@ -7145,7 +7164,7 @@
         <v>107</v>
       </c>
       <c r="AZ20" s="36" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="BA20" s="20">
         <v>19810411</v>
@@ -7253,7 +7272,7 @@
         <v>150</v>
       </c>
       <c r="DD20" s="22" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="2:108" ht="20" customHeight="1">
@@ -7390,7 +7409,7 @@
         <v>107</v>
       </c>
       <c r="AZ21" s="36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="BA21" s="20">
         <v>19810411</v>
@@ -7617,7 +7636,7 @@
         <v>107</v>
       </c>
       <c r="AZ22" s="36" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="BA22" s="20">
         <v>20170313</v>
@@ -7731,7 +7750,7 @@
         <v>150</v>
       </c>
       <c r="DD22" s="22" t="s">
-        <v>263</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="2:108" ht="20" customHeight="1">
@@ -7868,7 +7887,7 @@
         <v>107</v>
       </c>
       <c r="AZ23" s="37" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="BA23" s="25">
         <v>19980504</v>
@@ -7978,7 +7997,7 @@
         <v>150</v>
       </c>
       <c r="DD23" s="27" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="2:108" ht="20" customHeight="1">
@@ -8115,7 +8134,7 @@
         <v>107</v>
       </c>
       <c r="AZ24" s="37" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="BA24" s="25">
         <v>19980504</v>
@@ -8330,7 +8349,7 @@
         <v>107</v>
       </c>
       <c r="AZ25" s="37" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="BA25" s="25">
         <v>20150315</v>
@@ -8539,7 +8558,7 @@
         <v>107</v>
       </c>
       <c r="AZ26" s="37" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="BA26" s="25">
         <v>20150522</v>
@@ -8645,7 +8664,7 @@
         <v>150</v>
       </c>
       <c r="DD26" s="26" t="s">
-        <v>258</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="2:108" ht="20" customHeight="1">
@@ -8774,7 +8793,7 @@
         <v>107</v>
       </c>
       <c r="AZ27" s="37" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="BA27" s="25">
         <v>20151031</v>
@@ -8784,7 +8803,7 @@
         <v>107</v>
       </c>
       <c r="BD27" s="26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="BE27" s="26" t="s">
         <v>115</v>
@@ -8862,7 +8881,7 @@
         <v>146</v>
       </c>
       <c r="CX27" s="26" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="CY27" s="26" t="s">
         <v>195</v>
@@ -8880,7 +8899,7 @@
         <v>185</v>
       </c>
       <c r="DD27" s="26" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:108" ht="20" customHeight="1">
@@ -8907,7 +8926,7 @@
       <c r="L28" s="31"/>
       <c r="M28" s="30"/>
       <c r="N28" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O28" s="31"/>
       <c r="P28" s="30">
@@ -9017,7 +9036,7 @@
         <v>107</v>
       </c>
       <c r="AZ28" s="38" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="BA28" s="30">
         <v>19910411</v>
@@ -9029,13 +9048,13 @@
         <v>107</v>
       </c>
       <c r="BD28" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="BE28" s="31" t="s">
         <v>115</v>
       </c>
       <c r="BF28" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BG28" s="32"/>
       <c r="BH28" s="32"/>
@@ -9098,7 +9117,7 @@
         <v>108</v>
       </c>
       <c r="CS28" s="31" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="CT28" s="31" t="s">
         <v>156</v>
@@ -9113,13 +9132,13 @@
         <v>146</v>
       </c>
       <c r="CX28" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="CY28" s="31" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="CZ28" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="DA28" s="31" t="s">
         <v>156</v>
@@ -9131,7 +9150,7 @@
         <v>185</v>
       </c>
       <c r="DD28" s="31" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1">
@@ -9158,7 +9177,7 @@
       <c r="L29" s="31"/>
       <c r="M29" s="30"/>
       <c r="N29" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O29" s="31"/>
       <c r="P29" s="30">
@@ -9268,7 +9287,7 @@
         <v>173</v>
       </c>
       <c r="AZ29" s="38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="BA29" s="30">
         <v>19910411</v>
@@ -9280,13 +9299,13 @@
         <v>107</v>
       </c>
       <c r="BD29" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="BE29" s="31" t="s">
         <v>115</v>
       </c>
       <c r="BF29" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BG29" s="32"/>
       <c r="BH29" s="32"/>
@@ -9385,7 +9404,7 @@
       <c r="L30" s="31"/>
       <c r="M30" s="30"/>
       <c r="N30" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O30" s="31"/>
       <c r="P30" s="30">
@@ -9483,7 +9502,7 @@
         <v>107</v>
       </c>
       <c r="AV30" s="31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AW30" s="31" t="s">
         <v>171</v>
@@ -9495,7 +9514,7 @@
         <v>173</v>
       </c>
       <c r="AZ30" s="38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="BA30" s="30">
         <v>20140512</v>
@@ -9507,13 +9526,13 @@
         <v>107</v>
       </c>
       <c r="BD30" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="BE30" s="31" t="s">
         <v>131</v>
       </c>
       <c r="BF30" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BG30" s="32"/>
       <c r="BH30" s="32"/>
@@ -9576,7 +9595,7 @@
         <v>108</v>
       </c>
       <c r="CS30" s="31" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="CT30" s="31" t="s">
         <v>156</v>
@@ -9591,13 +9610,13 @@
         <v>146</v>
       </c>
       <c r="CX30" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="CY30" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="CZ30" s="31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="DA30" s="31" t="s">
         <v>156</v>
@@ -9606,10 +9625,10 @@
         <v>146</v>
       </c>
       <c r="DC30" s="31" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="DD30" s="31" t="s">
-        <v>266</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="2:108" ht="20" customHeight="1">
@@ -9636,7 +9655,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
       <c r="N31" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="10">
@@ -9746,7 +9765,7 @@
         <v>107</v>
       </c>
       <c r="AZ31" s="34" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="BA31" s="10">
         <v>19910411</v>
@@ -9827,13 +9846,13 @@
         <v>108</v>
       </c>
       <c r="CS31" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="CT31" s="11" t="s">
         <v>145</v>
       </c>
       <c r="CU31" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="CV31" s="11" t="s">
         <v>146</v>
@@ -9842,13 +9861,13 @@
         <v>146</v>
       </c>
       <c r="CX31" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="CY31" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="CZ31" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="DA31" s="11" t="s">
         <v>149</v>
@@ -9860,7 +9879,7 @@
         <v>150</v>
       </c>
       <c r="DD31" s="11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="2:108" ht="20" customHeight="1">
@@ -9887,7 +9906,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
       <c r="N32" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="10">
@@ -9997,7 +10016,7 @@
         <v>107</v>
       </c>
       <c r="AZ32" s="34" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BA32" s="10">
         <v>19910411</v>
@@ -10009,13 +10028,13 @@
         <v>107</v>
       </c>
       <c r="BD32" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="BE32" s="11" t="s">
         <v>115</v>
       </c>
       <c r="BF32" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="BG32" s="12"/>
       <c r="BH32" s="12"/>
@@ -10114,7 +10133,7 @@
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
       <c r="N33" s="26" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O33" s="26"/>
       <c r="P33" s="25">
@@ -10224,7 +10243,7 @@
         <v>107</v>
       </c>
       <c r="AZ33" s="37" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BA33" s="25">
         <v>20080410</v>
@@ -10310,13 +10329,13 @@
         <v>146</v>
       </c>
       <c r="CX33" s="26" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="CY33" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="CZ33" s="26" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="DA33" s="26" t="s">
         <v>149</v>
@@ -10328,7 +10347,7 @@
         <v>150</v>
       </c>
       <c r="DD33" s="26" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="2:108" ht="20" customHeight="1">
@@ -10355,7 +10374,7 @@
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="O34" s="16"/>
       <c r="P34" s="15">
@@ -10465,7 +10484,7 @@
         <v>107</v>
       </c>
       <c r="AZ34" s="35" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BA34" s="15">
         <v>20150214</v>
@@ -10553,13 +10572,13 @@
         <v>146</v>
       </c>
       <c r="CX34" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="CY34" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="CZ34" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="DA34" s="16" t="s">
         <v>149</v>
@@ -10571,7 +10590,7 @@
         <v>150</v>
       </c>
       <c r="DD34" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="2:108" ht="20" customHeight="1">
@@ -10598,7 +10617,7 @@
       <c r="L35" s="31"/>
       <c r="M35" s="30"/>
       <c r="N35" s="43" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O35" s="31"/>
       <c r="P35" s="30">
@@ -10696,7 +10715,7 @@
         <v>107</v>
       </c>
       <c r="AV35" s="31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AW35" s="31" t="s">
         <v>171</v>
@@ -10708,7 +10727,7 @@
         <v>173</v>
       </c>
       <c r="AZ35" s="38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="BA35" s="30">
         <v>20140512</v>
@@ -10720,13 +10739,13 @@
         <v>107</v>
       </c>
       <c r="BD35" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="BE35" s="31" t="s">
         <v>131</v>
       </c>
       <c r="BF35" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BG35" s="32"/>
       <c r="BH35" s="32"/>
@@ -10758,7 +10777,7 @@
         <v>140</v>
       </c>
       <c r="CF35" s="31" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="CG35" s="31" t="s">
         <v>108</v>
@@ -10789,7 +10808,7 @@
         <v>108</v>
       </c>
       <c r="CS35" s="31" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="CT35" s="31" t="s">
         <v>149</v>
@@ -10804,13 +10823,13 @@
         <v>146</v>
       </c>
       <c r="CX35" s="31" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="CY35" s="31" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="CZ35" s="31" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="DA35" s="31" t="s">
         <v>149</v>
@@ -10822,7 +10841,7 @@
         <v>150</v>
       </c>
       <c r="DD35" s="31" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update configurable flow e2e test for dismissByAge option
[#166587897]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28860" windowHeight="17600"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="271">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -810,15 +810,9 @@
     <t>04/11/1983</t>
   </si>
   <si>
-    <t>Reduce all 11359(C) HS convictions</t>
-  </si>
-  <si>
     <t>Dismiss all 11358 HS convictions</t>
   </si>
   <si>
-    <t>Reduce all 11357(B)HS convictions</t>
-  </si>
-  <si>
     <t>Reduce all 11359HS convictions</t>
   </si>
   <si>
@@ -835,6 +829,9 @@
   </si>
   <si>
     <t>21 years or younger</t>
+  </si>
+  <si>
+    <t>57 years or older</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1063,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1319,7 +1334,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1339,6 +1354,9 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1358,6 +1376,9 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2518,8 +2539,8 @@
   </sheetPr>
   <dimension ref="B1:DD35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CD3" workbookViewId="0">
-      <selection activeCell="CF35" sqref="CF35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CF1" workbookViewId="0">
+      <selection activeCell="DD17" sqref="DD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4464,7 +4485,7 @@
         <v>150</v>
       </c>
       <c r="DD8" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="2:108" ht="20" customHeight="1">
@@ -5393,10 +5414,10 @@
         <v>146</v>
       </c>
       <c r="DC12" s="26" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="DD12" s="26" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="2:108" ht="20" customHeight="1">
@@ -5870,7 +5891,7 @@
         <v>150</v>
       </c>
       <c r="DD14" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="2:108" ht="20" hidden="1" customHeight="1">
@@ -6572,10 +6593,10 @@
         <v>146</v>
       </c>
       <c r="DC17" s="17" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="DD17" s="17" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="2:108" ht="20" customHeight="1">
@@ -7272,7 +7293,7 @@
         <v>150</v>
       </c>
       <c r="DD20" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="2:108" ht="20" customHeight="1">
@@ -7997,7 +8018,7 @@
         <v>150</v>
       </c>
       <c r="DD23" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="2:108" ht="20" customHeight="1">
@@ -8899,7 +8920,7 @@
         <v>185</v>
       </c>
       <c r="DD27" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="2:108" ht="20" customHeight="1">
@@ -9150,7 +9171,7 @@
         <v>185</v>
       </c>
       <c r="DD28" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1">
@@ -9879,7 +9900,7 @@
         <v>150</v>
       </c>
       <c r="DD31" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="2:108" ht="20" customHeight="1">
@@ -10347,7 +10368,7 @@
         <v>150</v>
       </c>
       <c r="DD33" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="2:108" ht="20" customHeight="1">
@@ -10590,7 +10611,7 @@
         <v>150</v>
       </c>
       <c r="DD34" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="2:108" ht="20" customHeight="1">
@@ -10808,7 +10829,7 @@
         <v>108</v>
       </c>
       <c r="CS35" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="CT35" s="31" t="s">
         <v>149</v>
@@ -10823,13 +10844,13 @@
         <v>146</v>
       </c>
       <c r="CX35" s="31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="CY35" s="31" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="CZ35" s="31" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="DA35" s="31" t="s">
         <v>149</v>
@@ -10841,7 +10862,7 @@
         <v>150</v>
       </c>
       <c r="DD35" s="31" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dismiss convictions older than yearsSinceConvictionThreshold
[#166587954]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="274">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -573,9 +573,6 @@
     <t>266 PC;314(1) PC</t>
   </si>
   <si>
-    <t>2.7</t>
-  </si>
-  <si>
     <t>Eligible for Reduction</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t xml:space="preserve">        </t>
   </si>
   <si>
-    <t>03/12/2017</t>
-  </si>
-  <si>
     <t>A971951352</t>
   </si>
   <si>
@@ -832,6 +826,21 @@
   </si>
   <si>
     <t>57 years or older</t>
+  </si>
+  <si>
+    <t>03/05/2010</t>
+  </si>
+  <si>
+    <t>9.7</t>
+  </si>
+  <si>
+    <t>04/11/2004</t>
+  </si>
+  <si>
+    <t>15.6</t>
+  </si>
+  <si>
+    <t>Conviction occurred 10 years ago</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1072,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1334,7 +1379,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1357,6 +1402,12 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1379,6 +1430,12 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2539,8 +2596,8 @@
   </sheetPr>
   <dimension ref="B1:DD35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CF1" workbookViewId="0">
-      <selection activeCell="DD17" sqref="DD17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CW1" workbookViewId="0">
+      <selection activeCell="CZ23" sqref="CZ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2646,7 +2703,7 @@
   <sheetData>
     <row r="1" spans="2:108" s="42" customFormat="1" ht="27.75" customHeight="1">
       <c r="B1" s="39" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C1" s="40"/>
       <c r="D1" s="41"/>
@@ -2659,16 +2716,16 @@
       <c r="K1" s="41"/>
       <c r="L1" s="41"/>
       <c r="M1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Q1" s="41"/>
       <c r="R1" s="41"/>
@@ -2678,7 +2735,7 @@
       <c r="V1" s="41"/>
       <c r="W1" s="41"/>
       <c r="X1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Y1" s="41"/>
       <c r="Z1" s="41"/>
@@ -2695,12 +2752,12 @@
       <c r="AK1" s="41"/>
       <c r="AL1" s="41"/>
       <c r="AM1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AN1" s="41"/>
       <c r="AO1" s="41"/>
       <c r="AP1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AQ1" s="41"/>
       <c r="AR1" s="41"/>
@@ -2708,23 +2765,23 @@
       <c r="AT1" s="41"/>
       <c r="AU1" s="41"/>
       <c r="AV1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AW1" s="41"/>
       <c r="AX1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AY1" s="41"/>
       <c r="AZ1" s="41"/>
       <c r="BA1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BB1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BC1" s="41"/>
       <c r="BD1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BE1" s="41"/>
       <c r="BF1" s="41"/>
@@ -2752,71 +2809,71 @@
       <c r="CB1" s="41"/>
       <c r="CC1" s="41"/>
       <c r="CD1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CE1" s="41"/>
       <c r="CF1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CG1" s="41"/>
       <c r="CH1" s="41"/>
       <c r="CI1" s="41"/>
       <c r="CJ1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CK1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CL1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CM1" s="41"/>
       <c r="CN1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CO1" s="41"/>
       <c r="CP1" s="41"/>
       <c r="CQ1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CR1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CS1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CT1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CU1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CV1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CW1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CX1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CY1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="CZ1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="DA1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="DB1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="DC1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="DD1" s="41" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="2:108" ht="20.25" customHeight="1">
@@ -3276,7 +3333,7 @@
         <v>107</v>
       </c>
       <c r="AZ3" s="33" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="BA3" s="5">
         <v>19790525</v>
@@ -3493,7 +3550,7 @@
         <v>107</v>
       </c>
       <c r="AZ4" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="BA4" s="10">
         <v>19790601</v>
@@ -3720,7 +3777,7 @@
         <v>107</v>
       </c>
       <c r="AZ5" s="34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="BA5" s="10">
         <v>19810410</v>
@@ -3937,7 +3994,7 @@
         <v>107</v>
       </c>
       <c r="AZ6" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="BA6" s="10">
         <v>19810410</v>
@@ -4154,7 +4211,7 @@
         <v>107</v>
       </c>
       <c r="AZ7" s="34" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="BA7" s="10">
         <v>19810411</v>
@@ -4371,7 +4428,7 @@
         <v>107</v>
       </c>
       <c r="AZ8" s="34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="BA8" s="10">
         <v>19810411</v>
@@ -4485,7 +4542,7 @@
         <v>150</v>
       </c>
       <c r="DD8" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="2:108" ht="20" customHeight="1">
@@ -4622,7 +4679,7 @@
         <v>107</v>
       </c>
       <c r="AZ9" s="37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BA9" s="25">
         <v>19790525</v>
@@ -4839,7 +4896,7 @@
         <v>107</v>
       </c>
       <c r="AZ10" s="37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BA10" s="25">
         <v>19790601</v>
@@ -4941,7 +4998,7 @@
         <v>159</v>
       </c>
       <c r="CZ10" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="DA10" s="26" t="s">
         <v>145</v>
@@ -4953,7 +5010,7 @@
         <v>150</v>
       </c>
       <c r="DD10" s="26" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="2:108" ht="20" customHeight="1">
@@ -5090,7 +5147,7 @@
         <v>107</v>
       </c>
       <c r="AZ11" s="37" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BA11" s="25">
         <v>19790601</v>
@@ -5303,7 +5360,7 @@
         <v>107</v>
       </c>
       <c r="AZ12" s="37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BA12" s="25">
         <v>19851101</v>
@@ -5315,7 +5372,7 @@
         <v>107</v>
       </c>
       <c r="BD12" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="BE12" s="26" t="s">
         <v>115</v>
@@ -5399,13 +5456,13 @@
         <v>157</v>
       </c>
       <c r="CX12" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="CY12" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="CZ12" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="DA12" s="26" t="s">
         <v>145</v>
@@ -5417,7 +5474,7 @@
         <v>150</v>
       </c>
       <c r="DD12" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="2:108" ht="20" customHeight="1">
@@ -5554,7 +5611,7 @@
         <v>107</v>
       </c>
       <c r="AZ13" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BA13" s="25">
         <v>19851101</v>
@@ -5775,7 +5832,7 @@
         <v>107</v>
       </c>
       <c r="AZ14" s="35" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="BA14" s="15">
         <v>19810411</v>
@@ -5879,7 +5936,7 @@
         <v>148</v>
       </c>
       <c r="CZ14" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="DA14" s="16" t="s">
         <v>169</v>
@@ -5891,7 +5948,7 @@
         <v>150</v>
       </c>
       <c r="DD14" s="17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="2:108" ht="20" hidden="1" customHeight="1">
@@ -6028,7 +6085,7 @@
         <v>173</v>
       </c>
       <c r="AZ15" s="35" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="BA15" s="15">
         <v>19810411</v>
@@ -6255,7 +6312,7 @@
         <v>173</v>
       </c>
       <c r="AZ16" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="BA16" s="15">
         <v>19810411</v>
@@ -6482,7 +6539,7 @@
         <v>107</v>
       </c>
       <c r="AZ17" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="BA17" s="15">
         <v>19810411</v>
@@ -6578,13 +6635,13 @@
         <v>146</v>
       </c>
       <c r="CX17" s="16" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="CY17" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="CZ17" s="16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="DA17" s="16" t="s">
         <v>169</v>
@@ -6596,7 +6653,7 @@
         <v>150</v>
       </c>
       <c r="DD17" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="2:108" ht="20" customHeight="1">
@@ -6733,7 +6790,7 @@
         <v>107</v>
       </c>
       <c r="AZ18" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="BA18" s="15">
         <v>19810411</v>
@@ -6852,7 +6909,7 @@
       </c>
       <c r="O19" s="21"/>
       <c r="P19" s="20">
-        <v>19600514</v>
+        <v>19700514</v>
       </c>
       <c r="Q19" s="20"/>
       <c r="R19" s="21" t="s">
@@ -6928,7 +6985,7 @@
         <v>107</v>
       </c>
       <c r="AP19" s="20">
-        <v>19810411</v>
+        <v>20040411</v>
       </c>
       <c r="AQ19" s="21" t="s">
         <v>107</v>
@@ -6958,7 +7015,7 @@
         <v>107</v>
       </c>
       <c r="AZ19" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="BA19" s="20">
         <v>19810411</v>
@@ -7079,7 +7136,7 @@
       </c>
       <c r="O20" s="21"/>
       <c r="P20" s="20">
-        <v>19600514</v>
+        <v>19700514</v>
       </c>
       <c r="Q20" s="20"/>
       <c r="R20" s="21" t="s">
@@ -7155,7 +7212,7 @@
         <v>181</v>
       </c>
       <c r="AP20" s="20">
-        <v>19810411</v>
+        <v>20040411</v>
       </c>
       <c r="AQ20" s="21" t="s">
         <v>181</v>
@@ -7185,7 +7242,7 @@
         <v>107</v>
       </c>
       <c r="AZ20" s="36" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="BA20" s="20">
         <v>19810411</v>
@@ -7197,7 +7254,7 @@
         <v>107</v>
       </c>
       <c r="BD20" s="21" t="s">
-        <v>136</v>
+        <v>201</v>
       </c>
       <c r="BE20" s="22"/>
       <c r="BF20" s="22"/>
@@ -7275,13 +7332,13 @@
         <v>146</v>
       </c>
       <c r="CX20" s="21" t="s">
-        <v>147</v>
+        <v>271</v>
       </c>
       <c r="CY20" s="21" t="s">
-        <v>148</v>
+        <v>272</v>
       </c>
       <c r="CZ20" s="21" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="DA20" s="21" t="s">
         <v>145</v>
@@ -7293,7 +7350,7 @@
         <v>150</v>
       </c>
       <c r="DD20" s="22" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="2:108" ht="20" customHeight="1">
@@ -7324,7 +7381,7 @@
       </c>
       <c r="O21" s="21"/>
       <c r="P21" s="20">
-        <v>19600514</v>
+        <v>19700514</v>
       </c>
       <c r="Q21" s="20"/>
       <c r="R21" s="21" t="s">
@@ -7400,7 +7457,7 @@
         <v>107</v>
       </c>
       <c r="AP21" s="20">
-        <v>19810411</v>
+        <v>20040411</v>
       </c>
       <c r="AQ21" s="21" t="s">
         <v>107</v>
@@ -7430,7 +7487,7 @@
         <v>107</v>
       </c>
       <c r="AZ21" s="36" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="BA21" s="20">
         <v>19810411</v>
@@ -7474,10 +7531,10 @@
       <c r="CB21" s="22"/>
       <c r="CC21" s="22"/>
       <c r="CD21" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="CE21" s="21" t="s">
         <v>186</v>
-      </c>
-      <c r="CE21" s="21" t="s">
-        <v>187</v>
       </c>
       <c r="CF21" s="21" t="s">
         <v>118</v>
@@ -7551,7 +7608,7 @@
       </c>
       <c r="O22" s="21"/>
       <c r="P22" s="20">
-        <v>19600514</v>
+        <v>19700514</v>
       </c>
       <c r="Q22" s="20"/>
       <c r="R22" s="21" t="s">
@@ -7627,7 +7684,7 @@
         <v>107</v>
       </c>
       <c r="AP22" s="20">
-        <v>20170312</v>
+        <v>20040411</v>
       </c>
       <c r="AQ22" s="21" t="s">
         <v>107</v>
@@ -7657,7 +7714,7 @@
         <v>107</v>
       </c>
       <c r="AZ22" s="36" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="BA22" s="20">
         <v>20170313</v>
@@ -7704,7 +7761,7 @@
         <v>139</v>
       </c>
       <c r="CE22" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CF22" s="21" t="s">
         <v>134</v>
@@ -7753,13 +7810,13 @@
         <v>146</v>
       </c>
       <c r="CX22" s="21" t="s">
-        <v>188</v>
+        <v>271</v>
       </c>
       <c r="CY22" s="21" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="CZ22" s="21" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="DA22" s="21" t="s">
         <v>145</v>
@@ -7771,7 +7828,7 @@
         <v>150</v>
       </c>
       <c r="DD22" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="2:108" ht="20" customHeight="1">
@@ -7788,7 +7845,7 @@
         <v>108</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
@@ -7798,7 +7855,7 @@
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O23" s="26"/>
       <c r="P23" s="25">
@@ -7908,7 +7965,7 @@
         <v>107</v>
       </c>
       <c r="AZ23" s="37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="BA23" s="25">
         <v>19980504</v>
@@ -7952,10 +8009,10 @@
       <c r="CB23" s="27"/>
       <c r="CC23" s="27"/>
       <c r="CD23" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="CE23" s="26" t="s">
         <v>186</v>
-      </c>
-      <c r="CE23" s="26" t="s">
-        <v>187</v>
       </c>
       <c r="CF23" s="26" t="s">
         <v>118</v>
@@ -7988,10 +8045,10 @@
         <v>757392</v>
       </c>
       <c r="CT23" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="CU23" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="CV23" s="26" t="s">
         <v>146</v>
@@ -8000,13 +8057,13 @@
         <v>146</v>
       </c>
       <c r="CX23" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="CY23" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="CZ23" s="26" t="s">
         <v>193</v>
-      </c>
-      <c r="CY23" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="CZ23" s="26" t="s">
-        <v>195</v>
       </c>
       <c r="DA23" s="26" t="s">
         <v>156</v>
@@ -8018,7 +8075,7 @@
         <v>150</v>
       </c>
       <c r="DD23" s="27" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="2:108" ht="20" customHeight="1">
@@ -8035,7 +8092,7 @@
         <v>108</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
@@ -8045,7 +8102,7 @@
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O24" s="26"/>
       <c r="P24" s="25">
@@ -8155,7 +8212,7 @@
         <v>107</v>
       </c>
       <c r="AZ24" s="37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="BA24" s="25">
         <v>19980504</v>
@@ -8167,7 +8224,7 @@
         <v>107</v>
       </c>
       <c r="BD24" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="BE24" s="26" t="s">
         <v>115</v>
@@ -8199,10 +8256,10 @@
       <c r="CB24" s="27"/>
       <c r="CC24" s="27"/>
       <c r="CD24" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="CE24" s="26" t="s">
         <v>186</v>
-      </c>
-      <c r="CE24" s="26" t="s">
-        <v>187</v>
       </c>
       <c r="CF24" s="26" t="s">
         <v>118</v>
@@ -8258,7 +8315,7 @@
         <v>108</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
@@ -8268,7 +8325,7 @@
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
       <c r="N25" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O25" s="26"/>
       <c r="P25" s="25">
@@ -8370,7 +8427,7 @@
         <v>107</v>
       </c>
       <c r="AZ25" s="37" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="BA25" s="25">
         <v>20150315</v>
@@ -8467,7 +8524,7 @@
         <v>108</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
@@ -8477,7 +8534,7 @@
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
       <c r="N26" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O26" s="26"/>
       <c r="P26" s="25">
@@ -8579,7 +8636,7 @@
         <v>107</v>
       </c>
       <c r="AZ26" s="37" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="BA26" s="25">
         <v>20150522</v>
@@ -8655,10 +8712,10 @@
         <v>757392</v>
       </c>
       <c r="CT26" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="CU26" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="CV26" s="26" t="s">
         <v>146</v>
@@ -8667,13 +8724,13 @@
         <v>146</v>
       </c>
       <c r="CX26" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="CY26" s="26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="CZ26" s="26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="DA26" s="26" t="s">
         <v>156</v>
@@ -8685,7 +8742,7 @@
         <v>150</v>
       </c>
       <c r="DD26" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="2:108" ht="20" customHeight="1">
@@ -8702,7 +8759,7 @@
         <v>108</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
@@ -8712,7 +8769,7 @@
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
       <c r="N27" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O27" s="26"/>
       <c r="P27" s="25">
@@ -8814,7 +8871,7 @@
         <v>107</v>
       </c>
       <c r="AZ27" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="BA27" s="25">
         <v>20151031</v>
@@ -8824,7 +8881,7 @@
         <v>107</v>
       </c>
       <c r="BD27" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="BE27" s="26" t="s">
         <v>115</v>
@@ -8890,10 +8947,10 @@
         <v>757392</v>
       </c>
       <c r="CT27" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="CU27" s="26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="CV27" s="26" t="s">
         <v>146</v>
@@ -8902,13 +8959,13 @@
         <v>146</v>
       </c>
       <c r="CX27" s="26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="CY27" s="26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="CZ27" s="26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="DA27" s="26" t="s">
         <v>156</v>
@@ -8917,10 +8974,10 @@
         <v>146</v>
       </c>
       <c r="DC27" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="DD27" s="26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="2:108" ht="20" customHeight="1">
@@ -8947,7 +9004,7 @@
       <c r="L28" s="31"/>
       <c r="M28" s="30"/>
       <c r="N28" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O28" s="31"/>
       <c r="P28" s="30">
@@ -9027,7 +9084,7 @@
         <v>107</v>
       </c>
       <c r="AP28" s="30">
-        <v>19910411</v>
+        <v>20100305</v>
       </c>
       <c r="AQ28" s="31" t="s">
         <v>107</v>
@@ -9057,7 +9114,7 @@
         <v>107</v>
       </c>
       <c r="AZ28" s="38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="BA28" s="30">
         <v>19910411</v>
@@ -9069,13 +9126,13 @@
         <v>107</v>
       </c>
       <c r="BD28" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE28" s="31" t="s">
         <v>115</v>
       </c>
       <c r="BF28" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BG28" s="32"/>
       <c r="BH28" s="32"/>
@@ -9138,7 +9195,7 @@
         <v>108</v>
       </c>
       <c r="CS28" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="CT28" s="31" t="s">
         <v>156</v>
@@ -9153,13 +9210,13 @@
         <v>146</v>
       </c>
       <c r="CX28" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="CY28" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="CZ28" s="31" t="s">
         <v>206</v>
-      </c>
-      <c r="CY28" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="CZ28" s="31" t="s">
-        <v>208</v>
       </c>
       <c r="DA28" s="31" t="s">
         <v>156</v>
@@ -9168,10 +9225,10 @@
         <v>146</v>
       </c>
       <c r="DC28" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="DD28" s="31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1">
@@ -9198,7 +9255,7 @@
       <c r="L29" s="31"/>
       <c r="M29" s="30"/>
       <c r="N29" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O29" s="31"/>
       <c r="P29" s="30">
@@ -9308,7 +9365,7 @@
         <v>173</v>
       </c>
       <c r="AZ29" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="BA29" s="30">
         <v>19910411</v>
@@ -9320,13 +9377,13 @@
         <v>107</v>
       </c>
       <c r="BD29" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE29" s="31" t="s">
         <v>115</v>
       </c>
       <c r="BF29" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BG29" s="32"/>
       <c r="BH29" s="32"/>
@@ -9425,7 +9482,7 @@
       <c r="L30" s="31"/>
       <c r="M30" s="30"/>
       <c r="N30" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O30" s="31"/>
       <c r="P30" s="30">
@@ -9523,7 +9580,7 @@
         <v>107</v>
       </c>
       <c r="AV30" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AW30" s="31" t="s">
         <v>171</v>
@@ -9535,7 +9592,7 @@
         <v>173</v>
       </c>
       <c r="AZ30" s="38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BA30" s="30">
         <v>20140512</v>
@@ -9547,13 +9604,13 @@
         <v>107</v>
       </c>
       <c r="BD30" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE30" s="31" t="s">
         <v>131</v>
       </c>
       <c r="BF30" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BG30" s="32"/>
       <c r="BH30" s="32"/>
@@ -9616,7 +9673,7 @@
         <v>108</v>
       </c>
       <c r="CS30" s="31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="CT30" s="31" t="s">
         <v>156</v>
@@ -9631,13 +9688,13 @@
         <v>146</v>
       </c>
       <c r="CX30" s="31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="CY30" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="CZ30" s="31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="DA30" s="31" t="s">
         <v>156</v>
@@ -9649,7 +9706,7 @@
         <v>150</v>
       </c>
       <c r="DD30" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="2:108" ht="20" customHeight="1">
@@ -9676,7 +9733,7 @@
       <c r="L31" s="11"/>
       <c r="M31" s="11"/>
       <c r="N31" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="10">
@@ -9786,7 +9843,7 @@
         <v>107</v>
       </c>
       <c r="AZ31" s="34" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="BA31" s="10">
         <v>19910411</v>
@@ -9867,13 +9924,13 @@
         <v>108</v>
       </c>
       <c r="CS31" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="CT31" s="11" t="s">
         <v>145</v>
       </c>
       <c r="CU31" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="CV31" s="11" t="s">
         <v>146</v>
@@ -9882,13 +9939,13 @@
         <v>146</v>
       </c>
       <c r="CX31" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="CY31" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="CZ31" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="DA31" s="11" t="s">
         <v>149</v>
@@ -9900,7 +9957,7 @@
         <v>150</v>
       </c>
       <c r="DD31" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="2:108" ht="20" customHeight="1">
@@ -9927,7 +9984,7 @@
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
       <c r="N32" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="10">
@@ -10037,7 +10094,7 @@
         <v>107</v>
       </c>
       <c r="AZ32" s="34" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="BA32" s="10">
         <v>19910411</v>
@@ -10049,13 +10106,13 @@
         <v>107</v>
       </c>
       <c r="BD32" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="BE32" s="11" t="s">
         <v>115</v>
       </c>
       <c r="BF32" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BG32" s="12"/>
       <c r="BH32" s="12"/>
@@ -10154,7 +10211,7 @@
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
       <c r="N33" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O33" s="26"/>
       <c r="P33" s="25">
@@ -10264,7 +10321,7 @@
         <v>107</v>
       </c>
       <c r="AZ33" s="37" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="BA33" s="25">
         <v>20080410</v>
@@ -10350,13 +10407,13 @@
         <v>146</v>
       </c>
       <c r="CX33" s="26" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="CY33" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="CZ33" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="DA33" s="26" t="s">
         <v>149</v>
@@ -10368,7 +10425,7 @@
         <v>150</v>
       </c>
       <c r="DD33" s="26" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="2:108" ht="20" customHeight="1">
@@ -10395,7 +10452,7 @@
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O34" s="16"/>
       <c r="P34" s="15">
@@ -10505,7 +10562,7 @@
         <v>107</v>
       </c>
       <c r="AZ34" s="35" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="BA34" s="15">
         <v>20150214</v>
@@ -10593,13 +10650,13 @@
         <v>146</v>
       </c>
       <c r="CX34" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="CY34" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="CZ34" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="DA34" s="16" t="s">
         <v>149</v>
@@ -10611,7 +10668,7 @@
         <v>150</v>
       </c>
       <c r="DD34" s="16" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="2:108" ht="20" customHeight="1">
@@ -10638,7 +10695,7 @@
       <c r="L35" s="31"/>
       <c r="M35" s="30"/>
       <c r="N35" s="43" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O35" s="31"/>
       <c r="P35" s="30">
@@ -10736,7 +10793,7 @@
         <v>107</v>
       </c>
       <c r="AV35" s="31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AW35" s="31" t="s">
         <v>171</v>
@@ -10748,7 +10805,7 @@
         <v>173</v>
       </c>
       <c r="AZ35" s="38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="BA35" s="30">
         <v>20140512</v>
@@ -10760,13 +10817,13 @@
         <v>107</v>
       </c>
       <c r="BD35" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE35" s="31" t="s">
         <v>131</v>
       </c>
       <c r="BF35" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BG35" s="32"/>
       <c r="BH35" s="32"/>
@@ -10829,7 +10886,7 @@
         <v>108</v>
       </c>
       <c r="CS35" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="CT35" s="31" t="s">
         <v>149</v>
@@ -10844,13 +10901,13 @@
         <v>146</v>
       </c>
       <c r="CX35" s="31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="CY35" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="CZ35" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="DA35" s="31" t="s">
         <v>149</v>
@@ -10862,7 +10919,7 @@
         <v>150</v>
       </c>
       <c r="DD35" s="31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change eligibility reason language to indicate threshold
[#166587954]

Co-authored-by: Vraj Mohan <vraj@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB1CC8D-F714-124E-9467-122381265D78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -840,13 +846,13 @@
     <t>15.6</t>
   </si>
   <si>
-    <t>Conviction occurred 10 years ago</t>
+    <t>Conviction occurred 10 or more years ago</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2590,17 +2596,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:DD35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CW1" workbookViewId="0">
-      <selection activeCell="CZ23" sqref="CZ23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CW6" workbookViewId="0">
+      <selection activeCell="DC14" sqref="DC14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
@@ -2698,10 +2704,10 @@
     <col min="104" max="104" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="20.5" style="1" customWidth="1"/>
     <col min="106" max="107" width="25.83203125" style="1" customWidth="1"/>
-    <col min="108" max="108" width="29.83203125" style="1" customWidth="1"/>
+    <col min="108" max="108" width="32.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:108" s="42" customFormat="1" ht="27.75" customHeight="1">
+    <row r="1" spans="2:108" s="42" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="39" t="s">
         <v>253</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="2:108" ht="20.25" customHeight="1">
+    <row r="2" spans="2:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:108" ht="20.25" customHeight="1">
+    <row r="3" spans="2:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
@@ -3416,7 +3422,7 @@
       <c r="DC3" s="7"/>
       <c r="DD3" s="7"/>
     </row>
-    <row r="4" spans="2:108" ht="20" customHeight="1">
+    <row r="4" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
@@ -3643,7 +3649,7 @@
       <c r="DC4" s="12"/>
       <c r="DD4" s="12"/>
     </row>
-    <row r="5" spans="2:108" ht="20" customHeight="1">
+    <row r="5" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
         <v>107</v>
       </c>
@@ -3860,7 +3866,7 @@
       <c r="DC5" s="12"/>
       <c r="DD5" s="12"/>
     </row>
-    <row r="6" spans="2:108" ht="20" customHeight="1">
+    <row r="6" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4077,7 +4083,7 @@
       <c r="DC6" s="12"/>
       <c r="DD6" s="12"/>
     </row>
-    <row r="7" spans="2:108" ht="20" customHeight="1">
+    <row r="7" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="8" t="s">
         <v>107</v>
       </c>
@@ -4294,7 +4300,7 @@
       <c r="DC7" s="12"/>
       <c r="DD7" s="12"/>
     </row>
-    <row r="8" spans="2:108" ht="20" customHeight="1">
+    <row r="8" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
         <v>107</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="2:108" ht="20" customHeight="1">
+    <row r="9" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23" t="s">
         <v>107</v>
       </c>
@@ -4762,7 +4768,7 @@
       <c r="DC9" s="26"/>
       <c r="DD9" s="26"/>
     </row>
-    <row r="10" spans="2:108" ht="20" customHeight="1">
+    <row r="10" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="23" t="s">
         <v>107</v>
       </c>
@@ -5013,7 +5019,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="2:108" ht="20" customHeight="1">
+    <row r="11" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5226,7 +5232,7 @@
       <c r="DC11" s="26"/>
       <c r="DD11" s="26"/>
     </row>
-    <row r="12" spans="2:108" ht="20" customHeight="1">
+    <row r="12" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="23" t="s">
         <v>107</v>
       </c>
@@ -5477,7 +5483,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="13" spans="2:108" ht="20" customHeight="1">
+    <row r="13" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="23" t="s">
         <v>107</v>
       </c>
@@ -5698,7 +5704,7 @@
       <c r="DC13" s="26"/>
       <c r="DD13" s="26"/>
     </row>
-    <row r="14" spans="2:108" ht="20" customHeight="1">
+    <row r="14" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="13" t="s">
         <v>107</v>
       </c>
@@ -5951,7 +5957,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="2:108" ht="20" hidden="1" customHeight="1">
+    <row r="15" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="13" t="s">
         <v>107</v>
       </c>
@@ -6178,7 +6184,7 @@
       <c r="DC15" s="17"/>
       <c r="DD15" s="17"/>
     </row>
-    <row r="16" spans="2:108" ht="20" hidden="1" customHeight="1">
+    <row r="16" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="13" t="s">
         <v>107</v>
       </c>
@@ -6405,7 +6411,7 @@
       <c r="DC16" s="17"/>
       <c r="DD16" s="17"/>
     </row>
-    <row r="17" spans="2:108" ht="20" customHeight="1">
+    <row r="17" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="13" t="s">
         <v>107</v>
       </c>
@@ -6656,7 +6662,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="2:108" ht="20" customHeight="1">
+    <row r="18" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="13" t="s">
         <v>107</v>
       </c>
@@ -6881,7 +6887,7 @@
       <c r="DC18" s="17"/>
       <c r="DD18" s="17"/>
     </row>
-    <row r="19" spans="2:108" ht="20" customHeight="1">
+    <row r="19" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
@@ -7108,7 +7114,7 @@
       <c r="DC19" s="22"/>
       <c r="DD19" s="22"/>
     </row>
-    <row r="20" spans="2:108" ht="20" customHeight="1">
+    <row r="20" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="18" t="s">
         <v>181</v>
       </c>
@@ -7353,7 +7359,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="21" spans="2:108" ht="20" customHeight="1">
+    <row r="21" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="18" t="s">
         <v>107</v>
       </c>
@@ -7580,7 +7586,7 @@
       <c r="DC21" s="22"/>
       <c r="DD21" s="22"/>
     </row>
-    <row r="22" spans="2:108" ht="20" customHeight="1">
+    <row r="22" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
         <v>107</v>
       </c>
@@ -7831,7 +7837,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="2:108" ht="20" customHeight="1">
+    <row r="23" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="23" t="s">
         <v>107</v>
       </c>
@@ -8078,7 +8084,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="2:108" ht="20" customHeight="1">
+    <row r="24" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="23" t="s">
         <v>107</v>
       </c>
@@ -8301,7 +8307,7 @@
       <c r="DC24" s="27"/>
       <c r="DD24" s="27"/>
     </row>
-    <row r="25" spans="2:108" ht="20" customHeight="1">
+    <row r="25" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -8510,7 +8516,7 @@
       <c r="DC25" s="27"/>
       <c r="DD25" s="27"/>
     </row>
-    <row r="26" spans="2:108" ht="20" customHeight="1">
+    <row r="26" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="23" t="s">
         <v>107</v>
       </c>
@@ -8745,7 +8751,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="2:108" ht="20" customHeight="1">
+    <row r="27" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="23" t="s">
         <v>107</v>
       </c>
@@ -8980,7 +8986,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="2:108" ht="20" customHeight="1">
+    <row r="28" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="28" t="s">
         <v>107</v>
       </c>
@@ -9231,7 +9237,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1">
+    <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="28" t="s">
         <v>107</v>
       </c>
@@ -9458,7 +9464,7 @@
       <c r="DC29" s="32"/>
       <c r="DD29" s="32"/>
     </row>
-    <row r="30" spans="2:108" ht="20" customHeight="1">
+    <row r="30" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="28" t="s">
         <v>107</v>
       </c>
@@ -9709,7 +9715,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="2:108" ht="20" customHeight="1">
+    <row r="31" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="8" t="s">
         <v>107</v>
       </c>
@@ -9960,7 +9966,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="2:108" ht="20" customHeight="1">
+    <row r="32" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="8" t="s">
         <v>107</v>
       </c>
@@ -10187,7 +10193,7 @@
       <c r="DC32" s="12"/>
       <c r="DD32" s="12"/>
     </row>
-    <row r="33" spans="2:108" ht="20" customHeight="1">
+    <row r="33" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="23" t="s">
         <v>107</v>
       </c>
@@ -10428,7 +10434,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="2:108" ht="20" customHeight="1">
+    <row r="34" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="13" t="s">
         <v>107</v>
       </c>
@@ -10671,7 +10677,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="35" spans="2:108" ht="20" customHeight="1">
+    <row r="35" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="28" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Update test fixtures to include supjectHasOnlyProp64Charges
[#166588003]

Co-authored-by: Vraj Mohan <vraj@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB1CC8D-F714-124E-9467-122381265D78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B0DEE-AD8D-864B-BAA1-399714FE7363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -816,9 +816,6 @@
     <t>Reduce all 11359HS convictions</t>
   </si>
   <si>
-    <t>Reduce all 11359 HS convictions</t>
-  </si>
-  <si>
     <t>222344</t>
   </si>
   <si>
@@ -847,6 +844,9 @@
   </si>
   <si>
     <t>Conviction occurred 10 or more years ago</t>
+  </si>
+  <si>
+    <t>Only has 11357-60 charges</t>
   </si>
 </sst>
 </file>
@@ -2602,8 +2602,8 @@
   </sheetPr>
   <dimension ref="B1:DD35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CW6" workbookViewId="0">
-      <selection activeCell="DC14" sqref="DC14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DC30" sqref="DC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5480,7 +5480,7 @@
         <v>150</v>
       </c>
       <c r="DD12" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -6659,7 +6659,7 @@
         <v>150</v>
       </c>
       <c r="DD17" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -7338,13 +7338,13 @@
         <v>146</v>
       </c>
       <c r="CX20" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="CY20" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="CY20" s="21" t="s">
-        <v>272</v>
-      </c>
       <c r="CZ20" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="DA20" s="21" t="s">
         <v>145</v>
@@ -7356,7 +7356,7 @@
         <v>150</v>
       </c>
       <c r="DD20" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -7816,13 +7816,13 @@
         <v>146</v>
       </c>
       <c r="CX22" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="CY22" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="CY22" s="21" t="s">
-        <v>272</v>
-      </c>
       <c r="CZ22" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="DA22" s="21" t="s">
         <v>145</v>
@@ -9216,10 +9216,10 @@
         <v>146</v>
       </c>
       <c r="CX28" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="CY28" s="31" t="s">
         <v>269</v>
-      </c>
-      <c r="CY28" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="CZ28" s="31" t="s">
         <v>206</v>
@@ -9231,10 +9231,10 @@
         <v>146</v>
       </c>
       <c r="DC28" s="31" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="DD28" s="31" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
@@ -10892,7 +10892,7 @@
         <v>108</v>
       </c>
       <c r="CS35" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="CT35" s="31" t="s">
         <v>149</v>
@@ -10907,13 +10907,13 @@
         <v>146</v>
       </c>
       <c r="CX35" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="CY35" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="CY35" s="31" t="s">
-        <v>266</v>
-      </c>
       <c r="CZ35" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="DA35" s="31" t="s">
         <v>149</v>
@@ -10925,7 +10925,7 @@
         <v>150</v>
       </c>
       <c r="DD35" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Output the # of Prop64 convictions by section
[#164714666]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B0DEE-AD8D-864B-BAA1-399714FE7363}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="279">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -847,12 +841,27 @@
   </si>
   <si>
     <t>Only has 11357-60 charges</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t># of HS 11357 convictions</t>
+  </si>
+  <si>
+    <t># of HS 11358 convictions</t>
+  </si>
+  <si>
+    <t># of HS 11359 convictions</t>
+  </si>
+  <si>
+    <t># of HS 11360 convictions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1078,8 +1087,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1385,7 +1430,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1414,6 +1459,12 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1442,6 +1493,12 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2596,17 +2653,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:DD35"/>
+  <dimension ref="B1:DH35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DC30" sqref="DC30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CW4" workbookViewId="0">
+      <selection activeCell="DE35" sqref="DE35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
@@ -2702,12 +2759,12 @@
     <col min="102" max="102" width="12.5" style="1" customWidth="1"/>
     <col min="103" max="103" width="23.5" style="1" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="20.5" style="1" customWidth="1"/>
-    <col min="106" max="107" width="25.83203125" style="1" customWidth="1"/>
-    <col min="108" max="108" width="32.6640625" style="1" customWidth="1"/>
+    <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
+    <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
+    <col min="112" max="112" width="32.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:108" s="42" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:112" s="42" customFormat="1" ht="27.75" customHeight="1">
       <c r="B1" s="39" t="s">
         <v>253</v>
       </c>
@@ -2881,8 +2938,20 @@
       <c r="DD1" s="41" t="s">
         <v>252</v>
       </c>
+      <c r="DE1" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="DF1" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="DG1" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="DH1" s="41" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="2" spans="2:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:112" ht="20.25" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3196,16 +3265,28 @@
         <v>103</v>
       </c>
       <c r="DB2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="DD2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="DE2" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="DF2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DG2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DH2" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:108" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:112" ht="20.25" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
@@ -3418,11 +3499,15 @@
       <c r="CY3" s="6"/>
       <c r="CZ3" s="6"/>
       <c r="DA3" s="6"/>
-      <c r="DB3" s="7"/>
-      <c r="DC3" s="7"/>
-      <c r="DD3" s="7"/>
+      <c r="DB3" s="6"/>
+      <c r="DC3" s="6"/>
+      <c r="DD3" s="6"/>
+      <c r="DE3" s="6"/>
+      <c r="DF3" s="7"/>
+      <c r="DG3" s="7"/>
+      <c r="DH3" s="7"/>
     </row>
-    <row r="4" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:112" ht="20" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
@@ -3645,11 +3730,15 @@
       <c r="CY4" s="11"/>
       <c r="CZ4" s="11"/>
       <c r="DA4" s="11"/>
-      <c r="DB4" s="12"/>
-      <c r="DC4" s="12"/>
-      <c r="DD4" s="12"/>
+      <c r="DB4" s="11"/>
+      <c r="DC4" s="11"/>
+      <c r="DD4" s="11"/>
+      <c r="DE4" s="11"/>
+      <c r="DF4" s="12"/>
+      <c r="DG4" s="12"/>
+      <c r="DH4" s="12"/>
     </row>
-    <row r="5" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:112" ht="20" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>107</v>
       </c>
@@ -3862,11 +3951,15 @@
       <c r="CY5" s="11"/>
       <c r="CZ5" s="11"/>
       <c r="DA5" s="11"/>
-      <c r="DB5" s="12"/>
-      <c r="DC5" s="12"/>
-      <c r="DD5" s="12"/>
+      <c r="DB5" s="11"/>
+      <c r="DC5" s="11"/>
+      <c r="DD5" s="11"/>
+      <c r="DE5" s="11"/>
+      <c r="DF5" s="12"/>
+      <c r="DG5" s="12"/>
+      <c r="DH5" s="12"/>
     </row>
-    <row r="6" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:112" ht="20" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4079,11 +4172,15 @@
       <c r="CY6" s="11"/>
       <c r="CZ6" s="11"/>
       <c r="DA6" s="11"/>
-      <c r="DB6" s="12"/>
-      <c r="DC6" s="12"/>
-      <c r="DD6" s="12"/>
+      <c r="DB6" s="11"/>
+      <c r="DC6" s="11"/>
+      <c r="DD6" s="11"/>
+      <c r="DE6" s="11"/>
+      <c r="DF6" s="12"/>
+      <c r="DG6" s="12"/>
+      <c r="DH6" s="12"/>
     </row>
-    <row r="7" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:112" ht="20" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>107</v>
       </c>
@@ -4296,11 +4393,15 @@
       <c r="CY7" s="11"/>
       <c r="CZ7" s="11"/>
       <c r="DA7" s="11"/>
-      <c r="DB7" s="12"/>
-      <c r="DC7" s="12"/>
-      <c r="DD7" s="12"/>
+      <c r="DB7" s="11"/>
+      <c r="DC7" s="11"/>
+      <c r="DD7" s="11"/>
+      <c r="DE7" s="11"/>
+      <c r="DF7" s="12"/>
+      <c r="DG7" s="12"/>
+      <c r="DH7" s="12"/>
     </row>
-    <row r="8" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:112" ht="20" customHeight="1">
       <c r="B8" s="8" t="s">
         <v>107</v>
       </c>
@@ -4542,16 +4643,28 @@
         <v>149</v>
       </c>
       <c r="DB8" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD8" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE8" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF8" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="DC8" s="11" t="s">
+      <c r="DG8" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DD8" s="11" t="s">
+      <c r="DH8" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:112" ht="20" customHeight="1">
       <c r="B9" s="23" t="s">
         <v>107</v>
       </c>
@@ -4767,8 +4880,12 @@
       <c r="DB9" s="26"/>
       <c r="DC9" s="26"/>
       <c r="DD9" s="26"/>
+      <c r="DE9" s="26"/>
+      <c r="DF9" s="26"/>
+      <c r="DG9" s="26"/>
+      <c r="DH9" s="26"/>
     </row>
-    <row r="10" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:112" ht="20" customHeight="1">
       <c r="B10" s="23" t="s">
         <v>107</v>
       </c>
@@ -5010,16 +5127,28 @@
         <v>145</v>
       </c>
       <c r="DB10" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="DC10" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DD10" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE10" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF10" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DC10" s="26" t="s">
+      <c r="DG10" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DD10" s="26" t="s">
+      <c r="DH10" s="26" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:112" ht="20" customHeight="1">
       <c r="B11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5231,8 +5360,12 @@
       <c r="DB11" s="26"/>
       <c r="DC11" s="26"/>
       <c r="DD11" s="26"/>
+      <c r="DE11" s="26"/>
+      <c r="DF11" s="26"/>
+      <c r="DG11" s="26"/>
+      <c r="DH11" s="26"/>
     </row>
-    <row r="12" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:112" ht="20" customHeight="1">
       <c r="B12" s="23" t="s">
         <v>107</v>
       </c>
@@ -5474,16 +5607,28 @@
         <v>145</v>
       </c>
       <c r="DB12" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="DC12" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DD12" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE12" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF12" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DC12" s="26" t="s">
+      <c r="DG12" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DD12" s="26" t="s">
+      <c r="DH12" s="26" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:112" ht="20" customHeight="1">
       <c r="B13" s="23" t="s">
         <v>107</v>
       </c>
@@ -5703,8 +5848,12 @@
       <c r="DB13" s="26"/>
       <c r="DC13" s="26"/>
       <c r="DD13" s="26"/>
+      <c r="DE13" s="26"/>
+      <c r="DF13" s="26"/>
+      <c r="DG13" s="26"/>
+      <c r="DH13" s="26"/>
     </row>
-    <row r="14" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:112" ht="20" customHeight="1">
       <c r="B14" s="13" t="s">
         <v>107</v>
       </c>
@@ -5948,16 +6097,28 @@
         <v>169</v>
       </c>
       <c r="DB14" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC14" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD14" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE14" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF14" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DC14" s="17" t="s">
+      <c r="DG14" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="DD14" s="17" t="s">
+      <c r="DH14" s="17" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:112" ht="20" customHeight="1">
       <c r="B15" s="13" t="s">
         <v>107</v>
       </c>
@@ -6180,11 +6341,15 @@
       <c r="CY15" s="16"/>
       <c r="CZ15" s="16"/>
       <c r="DA15" s="16"/>
-      <c r="DB15" s="17"/>
-      <c r="DC15" s="17"/>
-      <c r="DD15" s="17"/>
+      <c r="DB15" s="16"/>
+      <c r="DC15" s="16"/>
+      <c r="DD15" s="16"/>
+      <c r="DE15" s="16"/>
+      <c r="DF15" s="17"/>
+      <c r="DG15" s="17"/>
+      <c r="DH15" s="17"/>
     </row>
-    <row r="16" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:112" ht="20" customHeight="1">
       <c r="B16" s="13" t="s">
         <v>107</v>
       </c>
@@ -6407,11 +6572,15 @@
       <c r="CY16" s="16"/>
       <c r="CZ16" s="16"/>
       <c r="DA16" s="16"/>
-      <c r="DB16" s="17"/>
-      <c r="DC16" s="17"/>
-      <c r="DD16" s="17"/>
+      <c r="DB16" s="16"/>
+      <c r="DC16" s="16"/>
+      <c r="DD16" s="16"/>
+      <c r="DE16" s="16"/>
+      <c r="DF16" s="17"/>
+      <c r="DG16" s="17"/>
+      <c r="DH16" s="17"/>
     </row>
-    <row r="17" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:112" ht="20" customHeight="1">
       <c r="B17" s="13" t="s">
         <v>107</v>
       </c>
@@ -6653,16 +6822,28 @@
         <v>169</v>
       </c>
       <c r="DB17" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC17" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD17" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE17" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF17" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DC17" s="17" t="s">
+      <c r="DG17" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="DD17" s="17" t="s">
+      <c r="DH17" s="17" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:112" ht="20" customHeight="1">
       <c r="B18" s="13" t="s">
         <v>107</v>
       </c>
@@ -6883,11 +7064,15 @@
       <c r="CY18" s="16"/>
       <c r="CZ18" s="16"/>
       <c r="DA18" s="16"/>
-      <c r="DB18" s="17"/>
-      <c r="DC18" s="17"/>
-      <c r="DD18" s="17"/>
+      <c r="DB18" s="16"/>
+      <c r="DC18" s="16"/>
+      <c r="DD18" s="16"/>
+      <c r="DE18" s="16"/>
+      <c r="DF18" s="17"/>
+      <c r="DG18" s="17"/>
+      <c r="DH18" s="17"/>
     </row>
-    <row r="19" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:112" ht="20" customHeight="1">
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
@@ -7110,11 +7295,15 @@
       <c r="CY19" s="21"/>
       <c r="CZ19" s="21"/>
       <c r="DA19" s="21"/>
-      <c r="DB19" s="22"/>
-      <c r="DC19" s="22"/>
-      <c r="DD19" s="22"/>
+      <c r="DB19" s="21"/>
+      <c r="DC19" s="21"/>
+      <c r="DD19" s="21"/>
+      <c r="DE19" s="21"/>
+      <c r="DF19" s="22"/>
+      <c r="DG19" s="22"/>
+      <c r="DH19" s="22"/>
     </row>
-    <row r="20" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:112" ht="20" customHeight="1">
       <c r="B20" s="18" t="s">
         <v>181</v>
       </c>
@@ -7350,16 +7539,28 @@
         <v>145</v>
       </c>
       <c r="DB20" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC20" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD20" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE20" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DC20" s="22" t="s">
+      <c r="DG20" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DD20" s="22" t="s">
+      <c r="DH20" s="22" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:112" ht="20" customHeight="1">
       <c r="B21" s="18" t="s">
         <v>107</v>
       </c>
@@ -7582,11 +7783,15 @@
       <c r="CY21" s="21"/>
       <c r="CZ21" s="21"/>
       <c r="DA21" s="21"/>
-      <c r="DB21" s="22"/>
-      <c r="DC21" s="22"/>
-      <c r="DD21" s="22"/>
+      <c r="DB21" s="21"/>
+      <c r="DC21" s="21"/>
+      <c r="DD21" s="21"/>
+      <c r="DE21" s="21"/>
+      <c r="DF21" s="22"/>
+      <c r="DG21" s="22"/>
+      <c r="DH21" s="22"/>
     </row>
-    <row r="22" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:112" ht="20" customHeight="1">
       <c r="B22" s="18" t="s">
         <v>107</v>
       </c>
@@ -7828,16 +8033,28 @@
         <v>145</v>
       </c>
       <c r="DB22" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE22" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DC22" s="22" t="s">
+      <c r="DG22" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DD22" s="22" t="s">
+      <c r="DH22" s="22" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:112" ht="20" customHeight="1">
       <c r="B23" s="23" t="s">
         <v>107</v>
       </c>
@@ -8075,16 +8292,28 @@
         <v>156</v>
       </c>
       <c r="DB23" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DC23" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD23" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE23" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF23" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DC23" s="27" t="s">
+      <c r="DG23" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="DD23" s="27" t="s">
+      <c r="DH23" s="27" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:112" ht="20" customHeight="1">
       <c r="B24" s="23" t="s">
         <v>107</v>
       </c>
@@ -8303,11 +8532,15 @@
       <c r="CY24" s="26"/>
       <c r="CZ24" s="26"/>
       <c r="DA24" s="26"/>
-      <c r="DB24" s="27"/>
-      <c r="DC24" s="27"/>
-      <c r="DD24" s="27"/>
+      <c r="DB24" s="26"/>
+      <c r="DC24" s="26"/>
+      <c r="DD24" s="26"/>
+      <c r="DE24" s="26"/>
+      <c r="DF24" s="27"/>
+      <c r="DG24" s="27"/>
+      <c r="DH24" s="27"/>
     </row>
-    <row r="25" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:112" ht="20" customHeight="1">
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -8512,11 +8745,15 @@
       <c r="CY25" s="26"/>
       <c r="CZ25" s="26"/>
       <c r="DA25" s="26"/>
-      <c r="DB25" s="27"/>
-      <c r="DC25" s="27"/>
-      <c r="DD25" s="27"/>
+      <c r="DB25" s="26"/>
+      <c r="DC25" s="26"/>
+      <c r="DD25" s="26"/>
+      <c r="DE25" s="26"/>
+      <c r="DF25" s="27"/>
+      <c r="DG25" s="27"/>
+      <c r="DH25" s="27"/>
     </row>
-    <row r="26" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:112" ht="20" customHeight="1">
       <c r="B26" s="23" t="s">
         <v>107</v>
       </c>
@@ -8742,16 +8979,28 @@
         <v>156</v>
       </c>
       <c r="DB26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DC26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE26" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF26" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DC26" s="26" t="s">
+      <c r="DG26" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DD26" s="26" t="s">
+      <c r="DH26" s="26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:112" ht="20" customHeight="1">
       <c r="B27" s="23" t="s">
         <v>107</v>
       </c>
@@ -8977,16 +9226,28 @@
         <v>156</v>
       </c>
       <c r="DB27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DC27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE27" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF27" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DC27" s="26" t="s">
+      <c r="DG27" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="DD27" s="26" t="s">
+      <c r="DH27" s="26" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:112" ht="20" customHeight="1">
       <c r="B28" s="28" t="s">
         <v>107</v>
       </c>
@@ -9228,16 +9489,28 @@
         <v>156</v>
       </c>
       <c r="DB28" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC28" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DD28" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="DE28" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF28" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DC28" s="31" t="s">
+      <c r="DG28" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DD28" s="31" t="s">
+      <c r="DH28" s="31" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="29" spans="2:108" ht="20" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:112" ht="20" customHeight="1">
       <c r="B29" s="28" t="s">
         <v>107</v>
       </c>
@@ -9460,11 +9733,15 @@
       <c r="CY29" s="31"/>
       <c r="CZ29" s="31"/>
       <c r="DA29" s="31"/>
-      <c r="DB29" s="32"/>
-      <c r="DC29" s="32"/>
-      <c r="DD29" s="32"/>
+      <c r="DB29" s="31"/>
+      <c r="DC29" s="31"/>
+      <c r="DD29" s="31"/>
+      <c r="DE29" s="31"/>
+      <c r="DF29" s="32"/>
+      <c r="DG29" s="32"/>
+      <c r="DH29" s="32"/>
     </row>
-    <row r="30" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:112" ht="20" customHeight="1">
       <c r="B30" s="28" t="s">
         <v>107</v>
       </c>
@@ -9706,16 +9983,28 @@
         <v>156</v>
       </c>
       <c r="DB30" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC30" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DD30" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="DE30" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF30" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DC30" s="31" t="s">
+      <c r="DG30" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DD30" s="31" t="s">
+      <c r="DH30" s="31" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:112" ht="20" customHeight="1">
       <c r="B31" s="8" t="s">
         <v>107</v>
       </c>
@@ -9957,16 +10246,28 @@
         <v>149</v>
       </c>
       <c r="DB31" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC31" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD31" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE31" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF31" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="DC31" s="11" t="s">
+      <c r="DG31" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DD31" s="11" t="s">
+      <c r="DH31" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:112" ht="20" customHeight="1">
       <c r="B32" s="8" t="s">
         <v>107</v>
       </c>
@@ -10189,11 +10490,15 @@
       <c r="CY32" s="11"/>
       <c r="CZ32" s="11"/>
       <c r="DA32" s="11"/>
-      <c r="DB32" s="12"/>
-      <c r="DC32" s="12"/>
-      <c r="DD32" s="12"/>
+      <c r="DB32" s="11"/>
+      <c r="DC32" s="11"/>
+      <c r="DD32" s="11"/>
+      <c r="DE32" s="11"/>
+      <c r="DF32" s="12"/>
+      <c r="DG32" s="12"/>
+      <c r="DH32" s="12"/>
     </row>
-    <row r="33" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:112" ht="20" customHeight="1">
       <c r="B33" s="23" t="s">
         <v>107</v>
       </c>
@@ -10425,16 +10730,28 @@
         <v>149</v>
       </c>
       <c r="DB33" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC33" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD33" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE33" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF33" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DC33" s="26" t="s">
+      <c r="DG33" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DD33" s="26" t="s">
+      <c r="DH33" s="26" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:112" ht="20" customHeight="1">
       <c r="B34" s="13" t="s">
         <v>107</v>
       </c>
@@ -10668,16 +10985,28 @@
         <v>149</v>
       </c>
       <c r="DB34" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC34" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="DD34" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE34" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF34" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DC34" s="16" t="s">
+      <c r="DG34" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DD34" s="16" t="s">
+      <c r="DH34" s="16" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="35" spans="2:108" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:112" ht="20" customHeight="1">
       <c r="B35" s="28" t="s">
         <v>107</v>
       </c>
@@ -10919,12 +11248,24 @@
         <v>149</v>
       </c>
       <c r="DB35" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DC35" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DD35" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE35" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="DF35" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DC35" s="31" t="s">
+      <c r="DG35" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DD35" s="31" t="s">
+      <c r="DH35" s="31" t="s">
         <v>266</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use regexes from predefined set
[#166891153]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="10800" windowWidth="51200" windowHeight="28340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -792,9 +792,6 @@
     <t>34.0</t>
   </si>
   <si>
-    <t>Dismiss all 11357(C)HS convictions</t>
-  </si>
-  <si>
     <t>11/01/1985</t>
   </si>
   <si>
@@ -804,12 +801,6 @@
     <t>04/11/1983</t>
   </si>
   <si>
-    <t>Dismiss all 11358 HS convictions</t>
-  </si>
-  <si>
-    <t>Reduce all 11359HS convictions</t>
-  </si>
-  <si>
     <t>222344</t>
   </si>
   <si>
@@ -856,6 +847,15 @@
   </si>
   <si>
     <t># of HS 11360 convictions</t>
+  </si>
+  <si>
+    <t>Dismiss all HS 11358 convictions</t>
+  </si>
+  <si>
+    <t>Dismiss all HS 11357(c) convictions</t>
+  </si>
+  <si>
+    <t>Reduce all HS 11359 convictions</t>
   </si>
 </sst>
 </file>
@@ -1087,8 +1087,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1430,7 +1436,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1465,6 +1471,7 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1499,6 +1506,7 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2659,8 +2667,8 @@
   </sheetPr>
   <dimension ref="B1:DH35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CW4" workbookViewId="0">
-      <selection activeCell="DE35" sqref="DE35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
+      <selection activeCell="DN32" sqref="DN32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3265,16 +3273,16 @@
         <v>103</v>
       </c>
       <c r="DB2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="DC2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="DD2" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="DE2" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="DC2" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="DD2" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="DF2" s="2" t="s">
         <v>104</v>
@@ -4643,16 +4651,16 @@
         <v>149</v>
       </c>
       <c r="DB8" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC8" s="11" t="s">
         <v>149</v>
       </c>
       <c r="DD8" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DE8" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF8" s="11" t="s">
         <v>104</v>
@@ -4661,7 +4669,7 @@
         <v>150</v>
       </c>
       <c r="DH8" s="11" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="2:112" ht="20" customHeight="1">
@@ -5130,13 +5138,13 @@
         <v>145</v>
       </c>
       <c r="DC10" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DD10" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DE10" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF10" s="26" t="s">
         <v>146</v>
@@ -5145,7 +5153,7 @@
         <v>150</v>
       </c>
       <c r="DH10" s="26" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="2:112" ht="20" customHeight="1">
@@ -5595,7 +5603,7 @@
         <v>157</v>
       </c>
       <c r="CX12" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="CY12" s="26" t="s">
         <v>256</v>
@@ -5610,13 +5618,13 @@
         <v>145</v>
       </c>
       <c r="DC12" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DD12" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DE12" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF12" s="26" t="s">
         <v>146</v>
@@ -5625,7 +5633,7 @@
         <v>150</v>
       </c>
       <c r="DH12" s="26" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="2:112" ht="20" customHeight="1">
@@ -6091,13 +6099,13 @@
         <v>148</v>
       </c>
       <c r="CZ14" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="DA14" s="16" t="s">
         <v>169</v>
       </c>
       <c r="DB14" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC14" s="16" t="s">
         <v>156</v>
@@ -6106,7 +6114,7 @@
         <v>149</v>
       </c>
       <c r="DE14" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF14" s="16" t="s">
         <v>146</v>
@@ -6115,7 +6123,7 @@
         <v>150</v>
       </c>
       <c r="DH14" s="17" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="2:112" ht="20" customHeight="1">
@@ -6810,19 +6818,19 @@
         <v>146</v>
       </c>
       <c r="CX17" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="CY17" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="CZ17" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="DA17" s="16" t="s">
         <v>169</v>
       </c>
       <c r="DB17" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC17" s="16" t="s">
         <v>156</v>
@@ -6831,7 +6839,7 @@
         <v>149</v>
       </c>
       <c r="DE17" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF17" s="16" t="s">
         <v>146</v>
@@ -6840,7 +6848,7 @@
         <v>150</v>
       </c>
       <c r="DH17" s="17" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="2:112" ht="20" customHeight="1">
@@ -7527,19 +7535,19 @@
         <v>146</v>
       </c>
       <c r="CX20" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="CY20" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="CZ20" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="DA20" s="21" t="s">
         <v>145</v>
       </c>
       <c r="DB20" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC20" s="21" t="s">
         <v>149</v>
@@ -7548,7 +7556,7 @@
         <v>149</v>
       </c>
       <c r="DE20" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF20" s="21" t="s">
         <v>146</v>
@@ -7557,7 +7565,7 @@
         <v>150</v>
       </c>
       <c r="DH20" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="2:112" ht="20" customHeight="1">
@@ -8021,19 +8029,19 @@
         <v>146</v>
       </c>
       <c r="CX22" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="CY22" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="CZ22" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="DA22" s="21" t="s">
         <v>145</v>
       </c>
       <c r="DB22" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC22" s="21" t="s">
         <v>149</v>
@@ -8042,7 +8050,7 @@
         <v>149</v>
       </c>
       <c r="DE22" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF22" s="21" t="s">
         <v>146</v>
@@ -8301,7 +8309,7 @@
         <v>149</v>
       </c>
       <c r="DE23" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF23" s="26" t="s">
         <v>146</v>
@@ -8310,7 +8318,7 @@
         <v>150</v>
       </c>
       <c r="DH23" s="27" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="2:112" ht="20" customHeight="1">
@@ -8988,7 +8996,7 @@
         <v>149</v>
       </c>
       <c r="DE26" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF26" s="26" t="s">
         <v>146</v>
@@ -9235,7 +9243,7 @@
         <v>149</v>
       </c>
       <c r="DE27" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF27" s="26" t="s">
         <v>146</v>
@@ -9244,7 +9252,7 @@
         <v>184</v>
       </c>
       <c r="DH27" s="26" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="2:112" ht="20" customHeight="1">
@@ -9477,10 +9485,10 @@
         <v>146</v>
       </c>
       <c r="CX28" s="31" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="CY28" s="31" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="CZ28" s="31" t="s">
         <v>206</v>
@@ -9489,16 +9497,16 @@
         <v>156</v>
       </c>
       <c r="DB28" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC28" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DD28" s="31" t="s">
         <v>156</v>
       </c>
       <c r="DE28" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF28" s="31" t="s">
         <v>146</v>
@@ -9507,7 +9515,7 @@
         <v>150</v>
       </c>
       <c r="DH28" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="2:112" ht="20" customHeight="1">
@@ -9983,16 +9991,16 @@
         <v>156</v>
       </c>
       <c r="DB30" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC30" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DD30" s="31" t="s">
         <v>156</v>
       </c>
       <c r="DE30" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF30" s="31" t="s">
         <v>146</v>
@@ -10246,16 +10254,16 @@
         <v>149</v>
       </c>
       <c r="DB31" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC31" s="11" t="s">
         <v>149</v>
       </c>
       <c r="DD31" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DE31" s="11" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF31" s="11" t="s">
         <v>146</v>
@@ -10264,7 +10272,7 @@
         <v>150</v>
       </c>
       <c r="DH31" s="11" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="2:112" ht="20" customHeight="1">
@@ -10730,16 +10738,16 @@
         <v>149</v>
       </c>
       <c r="DB33" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC33" s="26" t="s">
         <v>149</v>
       </c>
       <c r="DD33" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DE33" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF33" s="26" t="s">
         <v>146</v>
@@ -10748,7 +10756,7 @@
         <v>150</v>
       </c>
       <c r="DH33" s="26" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="2:112" ht="20" customHeight="1">
@@ -10985,16 +10993,16 @@
         <v>149</v>
       </c>
       <c r="DB34" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC34" s="16" t="s">
         <v>149</v>
       </c>
       <c r="DD34" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DE34" s="16" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF34" s="16" t="s">
         <v>146</v>
@@ -11003,7 +11011,7 @@
         <v>150</v>
       </c>
       <c r="DH34" s="16" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="2:112" ht="20" customHeight="1">
@@ -11221,7 +11229,7 @@
         <v>108</v>
       </c>
       <c r="CS35" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="CT35" s="31" t="s">
         <v>149</v>
@@ -11236,28 +11244,28 @@
         <v>146</v>
       </c>
       <c r="CX35" s="31" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="CY35" s="31" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="CZ35" s="31" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="DA35" s="31" t="s">
         <v>149</v>
       </c>
       <c r="DB35" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DC35" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DD35" s="31" t="s">
         <v>149</v>
       </c>
       <c r="DE35" s="31" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="DF35" s="31" t="s">
         <v>146</v>
@@ -11266,7 +11274,7 @@
         <v>150</v>
       </c>
       <c r="DH35" s="31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dismiss/Reduce 11357 convictions when no subsection is specified
[#166851482]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10800" windowWidth="51200" windowHeight="28340"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="284">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -856,6 +856,21 @@
   </si>
   <si>
     <t>Reduce all HS 11359 convictions</t>
+  </si>
+  <si>
+    <t>MAUL, DARTH</t>
+  </si>
+  <si>
+    <t>11357 HS-NO SPECIFIED SUBSECTION</t>
+  </si>
+  <si>
+    <t>07/03/2012</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>Dismiss all HS 11357 convictions (when no sub-section is specified)</t>
   </si>
 </sst>
 </file>
@@ -894,7 +909,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,12 +950,6 @@
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1087,7 +1096,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1301,8 +1310,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1432,11 +1447,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1472,6 +1484,7 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1507,6 +1520,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2665,10 +2679,10 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:DH35"/>
+  <dimension ref="B1:DH36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
-      <selection activeCell="DN32" sqref="DN32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CR1" workbookViewId="0">
+      <selection activeCell="CS33" sqref="CS33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2769,7 +2783,7 @@
     <col min="104" max="104" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
     <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
-    <col min="112" max="112" width="32.6640625" style="1" customWidth="1"/>
+    <col min="112" max="112" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:112" s="42" customFormat="1" ht="27.75" customHeight="1">
@@ -11015,266 +11029,529 @@
       </c>
     </row>
     <row r="35" spans="2:112" ht="20" customHeight="1">
-      <c r="B35" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" s="30">
+      <c r="B35" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="20">
         <v>21345614</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F35" s="30">
+      <c r="F35" s="20">
         <v>1008743215</v>
       </c>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="43" t="s">
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="O35" s="31"/>
-      <c r="P35" s="30">
+      <c r="O35" s="21"/>
+      <c r="P35" s="20">
         <v>19800514</v>
       </c>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="31" t="s">
+      <c r="Q35" s="20"/>
+      <c r="R35" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="S35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="T35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="U35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="V35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="W35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="X35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM35" s="31" t="s">
+      <c r="S35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="U35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="V35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="W35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="X35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM35" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AN35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP35" s="30">
+      <c r="AN35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP35" s="20">
         <v>19940912</v>
       </c>
-      <c r="AQ35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AR35" s="31" t="s">
+      <c r="AQ35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR35" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="AS35" s="31" t="s">
+      <c r="AS35" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="AT35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV35" s="31" t="s">
+      <c r="AT35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV35" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="AW35" s="31" t="s">
+      <c r="AW35" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="AX35" s="31" t="s">
+      <c r="AX35" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AY35" s="31" t="s">
+      <c r="AY35" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="AZ35" s="38" t="s">
+      <c r="AZ35" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="BA35" s="30">
+      <c r="BA35" s="20">
         <v>20140512</v>
       </c>
-      <c r="BB35" s="30">
+      <c r="BB35" s="20">
         <v>222344</v>
       </c>
-      <c r="BC35" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="BD35" s="31" t="s">
+      <c r="BC35" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD35" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="BE35" s="31" t="s">
+      <c r="BE35" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="BF35" s="31" t="s">
+      <c r="BF35" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="BG35" s="32"/>
-      <c r="BH35" s="32"/>
-      <c r="BI35" s="32"/>
-      <c r="BJ35" s="32"/>
-      <c r="BK35" s="32"/>
-      <c r="BL35" s="32"/>
-      <c r="BM35" s="32"/>
-      <c r="BN35" s="32"/>
-      <c r="BO35" s="32"/>
-      <c r="BP35" s="32"/>
-      <c r="BQ35" s="32"/>
-      <c r="BR35" s="32"/>
-      <c r="BS35" s="32"/>
-      <c r="BT35" s="32"/>
-      <c r="BU35" s="32"/>
-      <c r="BV35" s="32"/>
-      <c r="BW35" s="32"/>
-      <c r="BX35" s="32"/>
-      <c r="BY35" s="32"/>
-      <c r="BZ35" s="32"/>
-      <c r="CA35" s="32"/>
-      <c r="CB35" s="32"/>
-      <c r="CC35" s="32"/>
-      <c r="CD35" s="31" t="s">
+      <c r="BG35" s="22"/>
+      <c r="BH35" s="22"/>
+      <c r="BI35" s="22"/>
+      <c r="BJ35" s="22"/>
+      <c r="BK35" s="22"/>
+      <c r="BL35" s="22"/>
+      <c r="BM35" s="22"/>
+      <c r="BN35" s="22"/>
+      <c r="BO35" s="22"/>
+      <c r="BP35" s="22"/>
+      <c r="BQ35" s="22"/>
+      <c r="BR35" s="22"/>
+      <c r="BS35" s="22"/>
+      <c r="BT35" s="22"/>
+      <c r="BU35" s="22"/>
+      <c r="BV35" s="22"/>
+      <c r="BW35" s="22"/>
+      <c r="BX35" s="22"/>
+      <c r="BY35" s="22"/>
+      <c r="BZ35" s="22"/>
+      <c r="CA35" s="22"/>
+      <c r="CB35" s="22"/>
+      <c r="CC35" s="22"/>
+      <c r="CD35" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="CE35" s="31" t="s">
+      <c r="CE35" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="CF35" s="31" t="s">
+      <c r="CF35" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="CG35" s="31" t="s">
+      <c r="CG35" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="CH35" s="32"/>
-      <c r="CI35" s="31" t="s">
+      <c r="CH35" s="22"/>
+      <c r="CI35" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="CJ35" s="31" t="s">
+      <c r="CJ35" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="CK35" s="30">
+      <c r="CK35" s="20">
         <v>6</v>
       </c>
-      <c r="CL35" s="31" t="s">
+      <c r="CL35" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="CM35" s="31" t="s">
+      <c r="CM35" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="CN35" s="30">
+      <c r="CN35" s="20">
         <v>25</v>
       </c>
-      <c r="CO35" s="32"/>
-      <c r="CP35" s="32"/>
-      <c r="CQ35" s="32"/>
-      <c r="CR35" s="31" t="s">
+      <c r="CO35" s="22"/>
+      <c r="CP35" s="22"/>
+      <c r="CQ35" s="22"/>
+      <c r="CR35" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="CS35" s="31" t="s">
+      <c r="CS35" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="CT35" s="31" t="s">
+      <c r="CT35" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="CU35" s="31" t="s">
+      <c r="CU35" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CV35" s="31" t="s">
+      <c r="CV35" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CW35" s="31" t="s">
+      <c r="CW35" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CX35" s="31" t="s">
+      <c r="CX35" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="CY35" s="31" t="s">
+      <c r="CY35" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="CZ35" s="31" t="s">
+      <c r="CZ35" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="DA35" s="31" t="s">
+      <c r="DA35" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="DB35" s="31" t="s">
+      <c r="DB35" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="DC35" s="31" t="s">
+      <c r="DC35" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="DD35" s="31" t="s">
+      <c r="DD35" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="DE35" s="31" t="s">
+      <c r="DE35" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="DF35" s="31" t="s">
+      <c r="DF35" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DG35" s="31" t="s">
+      <c r="DG35" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DH35" s="31" t="s">
+      <c r="DH35" s="22" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="2:112" ht="20" customHeight="1">
+      <c r="B36" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="25">
+        <v>313456</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36" s="26">
+        <v>1008743215</v>
+      </c>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="O36" s="26"/>
+      <c r="P36" s="25">
+        <v>19820513</v>
+      </c>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="S36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="U36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="V36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="W36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="X36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM36" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP36" s="25">
+        <v>20120703</v>
+      </c>
+      <c r="AQ36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR36" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS36" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV36" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW36" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX36" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY36" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="AZ36" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA36" s="25">
+        <v>20140512</v>
+      </c>
+      <c r="BB36" s="25">
+        <v>222344</v>
+      </c>
+      <c r="BC36" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD36" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="BE36" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF36" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG36" s="27"/>
+      <c r="BH36" s="27"/>
+      <c r="BI36" s="27"/>
+      <c r="BJ36" s="27"/>
+      <c r="BK36" s="27"/>
+      <c r="BL36" s="27"/>
+      <c r="BM36" s="27"/>
+      <c r="BN36" s="27"/>
+      <c r="BO36" s="27"/>
+      <c r="BP36" s="27"/>
+      <c r="BQ36" s="27"/>
+      <c r="BR36" s="27"/>
+      <c r="BS36" s="27"/>
+      <c r="BT36" s="27"/>
+      <c r="BU36" s="27"/>
+      <c r="BV36" s="27"/>
+      <c r="BW36" s="27"/>
+      <c r="BX36" s="27"/>
+      <c r="BY36" s="27"/>
+      <c r="BZ36" s="27"/>
+      <c r="CA36" s="27"/>
+      <c r="CB36" s="27"/>
+      <c r="CC36" s="27"/>
+      <c r="CD36" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="CE36" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="CF36" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="CG36" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH36" s="27"/>
+      <c r="CI36" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="CJ36" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="CK36" s="25">
+        <v>6</v>
+      </c>
+      <c r="CL36" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="CM36" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="CN36" s="27">
+        <v>25</v>
+      </c>
+      <c r="CO36" s="27"/>
+      <c r="CP36" s="27"/>
+      <c r="CQ36" s="27"/>
+      <c r="CR36" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS36" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="CT36" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="CU36" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CV36" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CW36" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CX36" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="CY36" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="CZ36" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="DA36" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DB36" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DC36" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="DD36" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="DE36" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="DF36" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG36" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="DH36" s="26" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more testing for deceased
[#167405606]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D094EB-54BE-5E4C-9813-1BAF24E11A00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="290">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -871,12 +877,30 @@
   </si>
   <si>
     <t>Dismiss all HS 11357 convictions (when no sub-section is specified)</t>
+  </si>
+  <si>
+    <t>Individual is deceased</t>
+  </si>
+  <si>
+    <t>11359 HS-CULTIVATE CANNABIS</t>
+  </si>
+  <si>
+    <t>101001032000</t>
+  </si>
+  <si>
+    <t>101001033000</t>
+  </si>
+  <si>
+    <t>555 PC-UH OH</t>
+  </si>
+  <si>
+    <t>3.7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2675,17 +2699,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:DH36"/>
+  <dimension ref="B1:DH38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CR1" workbookViewId="0">
-      <selection activeCell="CS33" sqref="CS33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CT1" workbookViewId="0">
+      <selection activeCell="DA48" sqref="DA48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
@@ -2739,37 +2763,37 @@
     <col min="55" max="55" width="14.83203125" style="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
     <col min="57" max="57" width="13.6640625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="19.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="20.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="23.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="21.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="20.5" style="1" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="21.5" style="1" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="19.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="24.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="69" max="69" width="17.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="20" style="1" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="73" max="74" width="17.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="75" max="77" width="16.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="78" max="78" width="18" style="1" hidden="1" customWidth="1"/>
-    <col min="79" max="79" width="17.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="12.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="81" max="81" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="18.6640625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="19.6640625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6640625" style="1" customWidth="1"/>
+    <col min="61" max="61" width="18.33203125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="23.33203125" style="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6640625" style="1" customWidth="1"/>
+    <col min="64" max="64" width="20.5" style="1" customWidth="1"/>
+    <col min="65" max="65" width="21.5" style="1" customWidth="1"/>
+    <col min="66" max="66" width="19.33203125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="24.33203125" style="1" customWidth="1"/>
+    <col min="68" max="68" width="15.1640625" style="1" customWidth="1"/>
+    <col min="69" max="69" width="17.1640625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="20" style="1" customWidth="1"/>
+    <col min="71" max="71" width="13" style="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" style="1" customWidth="1"/>
+    <col min="73" max="74" width="17.1640625" style="1" customWidth="1"/>
+    <col min="75" max="77" width="16.6640625" style="1" customWidth="1"/>
+    <col min="78" max="78" width="18" style="1" customWidth="1"/>
+    <col min="79" max="79" width="17.6640625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="12.1640625" style="1" customWidth="1"/>
+    <col min="81" max="81" width="11" style="1" customWidth="1"/>
     <col min="82" max="82" width="26.33203125" style="1" customWidth="1"/>
     <col min="83" max="83" width="16.83203125" style="1" customWidth="1"/>
     <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
-    <col min="85" max="85" width="14.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="87" max="87" width="16" style="1" hidden="1" customWidth="1"/>
-    <col min="88" max="88" width="16.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="90" max="90" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
+    <col min="87" max="87" width="16" style="1" customWidth="1"/>
+    <col min="88" max="88" width="16.83203125" style="1" customWidth="1"/>
+    <col min="89" max="89" width="13.5" style="1" customWidth="1"/>
+    <col min="90" max="90" width="16.5" style="1" customWidth="1"/>
+    <col min="91" max="91" width="17.33203125" style="1" customWidth="1"/>
     <col min="92" max="92" width="9.33203125" style="1" customWidth="1"/>
     <col min="93" max="93" width="8.83203125" style="1" customWidth="1"/>
     <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
@@ -2779,14 +2803,14 @@
     <col min="98" max="98" width="24" style="1" customWidth="1"/>
     <col min="99" max="101" width="23.6640625" style="1" customWidth="1"/>
     <col min="102" max="102" width="12.5" style="1" customWidth="1"/>
-    <col min="103" max="103" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="23.5" style="1" customWidth="1"/>
+    <col min="104" max="104" width="23.1640625" style="1" customWidth="1"/>
     <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
     <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
     <col min="112" max="112" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:112" s="42" customFormat="1" ht="27.75" customHeight="1">
+    <row r="1" spans="2:112" s="42" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="39" t="s">
         <v>253</v>
       </c>
@@ -2973,7 +2997,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="2:112" ht="20.25" customHeight="1">
+    <row r="2" spans="2:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3308,7 +3332,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:112" ht="20.25" customHeight="1">
+    <row r="3" spans="2:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
@@ -3529,7 +3553,7 @@
       <c r="DG3" s="7"/>
       <c r="DH3" s="7"/>
     </row>
-    <row r="4" spans="2:112" ht="20" customHeight="1">
+    <row r="4" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
@@ -3760,7 +3784,7 @@
       <c r="DG4" s="12"/>
       <c r="DH4" s="12"/>
     </row>
-    <row r="5" spans="2:112" ht="20" customHeight="1">
+    <row r="5" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
         <v>107</v>
       </c>
@@ -3981,7 +4005,7 @@
       <c r="DG5" s="12"/>
       <c r="DH5" s="12"/>
     </row>
-    <row r="6" spans="2:112" ht="20" customHeight="1">
+    <row r="6" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4202,7 +4226,7 @@
       <c r="DG6" s="12"/>
       <c r="DH6" s="12"/>
     </row>
-    <row r="7" spans="2:112" ht="20" customHeight="1">
+    <row r="7" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="8" t="s">
         <v>107</v>
       </c>
@@ -4423,7 +4447,7 @@
       <c r="DG7" s="12"/>
       <c r="DH7" s="12"/>
     </row>
-    <row r="8" spans="2:112" ht="20" customHeight="1">
+    <row r="8" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="8" t="s">
         <v>107</v>
       </c>
@@ -4686,7 +4710,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="2:112" ht="20" customHeight="1">
+    <row r="9" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23" t="s">
         <v>107</v>
       </c>
@@ -4907,7 +4931,7 @@
       <c r="DG9" s="26"/>
       <c r="DH9" s="26"/>
     </row>
-    <row r="10" spans="2:112" ht="20" customHeight="1">
+    <row r="10" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="23" t="s">
         <v>107</v>
       </c>
@@ -5170,7 +5194,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="2:112" ht="20" customHeight="1">
+    <row r="11" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5387,7 +5411,7 @@
       <c r="DG11" s="26"/>
       <c r="DH11" s="26"/>
     </row>
-    <row r="12" spans="2:112" ht="20" customHeight="1">
+    <row r="12" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="23" t="s">
         <v>107</v>
       </c>
@@ -5650,7 +5674,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="2:112" ht="20" customHeight="1">
+    <row r="13" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="23" t="s">
         <v>107</v>
       </c>
@@ -5875,7 +5899,7 @@
       <c r="DG13" s="26"/>
       <c r="DH13" s="26"/>
     </row>
-    <row r="14" spans="2:112" ht="20" customHeight="1">
+    <row r="14" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="13" t="s">
         <v>107</v>
       </c>
@@ -6140,7 +6164,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="2:112" ht="20" customHeight="1">
+    <row r="15" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="13" t="s">
         <v>107</v>
       </c>
@@ -6371,7 +6395,7 @@
       <c r="DG15" s="17"/>
       <c r="DH15" s="17"/>
     </row>
-    <row r="16" spans="2:112" ht="20" customHeight="1">
+    <row r="16" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="13" t="s">
         <v>107</v>
       </c>
@@ -6602,7 +6626,7 @@
       <c r="DG16" s="17"/>
       <c r="DH16" s="17"/>
     </row>
-    <row r="17" spans="2:112" ht="20" customHeight="1">
+    <row r="17" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="13" t="s">
         <v>107</v>
       </c>
@@ -6865,7 +6889,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="2:112" ht="20" customHeight="1">
+    <row r="18" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="13" t="s">
         <v>107</v>
       </c>
@@ -7094,7 +7118,7 @@
       <c r="DG18" s="17"/>
       <c r="DH18" s="17"/>
     </row>
-    <row r="19" spans="2:112" ht="20" customHeight="1">
+    <row r="19" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
@@ -7325,7 +7349,7 @@
       <c r="DG19" s="22"/>
       <c r="DH19" s="22"/>
     </row>
-    <row r="20" spans="2:112" ht="20" customHeight="1">
+    <row r="20" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="18" t="s">
         <v>181</v>
       </c>
@@ -7582,7 +7606,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="2:112" ht="20" customHeight="1">
+    <row r="21" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="18" t="s">
         <v>107</v>
       </c>
@@ -7813,7 +7837,7 @@
       <c r="DG21" s="22"/>
       <c r="DH21" s="22"/>
     </row>
-    <row r="22" spans="2:112" ht="20" customHeight="1">
+    <row r="22" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="18" t="s">
         <v>107</v>
       </c>
@@ -8076,7 +8100,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="2:112" ht="20" customHeight="1">
+    <row r="23" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="23" t="s">
         <v>107</v>
       </c>
@@ -8335,7 +8359,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="2:112" ht="20" customHeight="1">
+    <row r="24" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="23" t="s">
         <v>107</v>
       </c>
@@ -8562,7 +8586,7 @@
       <c r="DG24" s="27"/>
       <c r="DH24" s="27"/>
     </row>
-    <row r="25" spans="2:112" ht="20" customHeight="1">
+    <row r="25" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -8775,7 +8799,7 @@
       <c r="DG25" s="27"/>
       <c r="DH25" s="27"/>
     </row>
-    <row r="26" spans="2:112" ht="20" customHeight="1">
+    <row r="26" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="23" t="s">
         <v>107</v>
       </c>
@@ -9022,7 +9046,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="2:112" ht="20" customHeight="1">
+    <row r="27" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="23" t="s">
         <v>107</v>
       </c>
@@ -9269,7 +9293,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="28" spans="2:112" ht="20" customHeight="1">
+    <row r="28" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="28" t="s">
         <v>107</v>
       </c>
@@ -9532,7 +9556,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="29" spans="2:112" ht="20" customHeight="1">
+    <row r="29" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="28" t="s">
         <v>107</v>
       </c>
@@ -9763,7 +9787,7 @@
       <c r="DG29" s="32"/>
       <c r="DH29" s="32"/>
     </row>
-    <row r="30" spans="2:112" ht="20" customHeight="1">
+    <row r="30" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="28" t="s">
         <v>107</v>
       </c>
@@ -10026,7 +10050,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="2:112" ht="20" customHeight="1">
+    <row r="31" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="8" t="s">
         <v>107</v>
       </c>
@@ -10289,7 +10313,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="32" spans="2:112" ht="20" customHeight="1">
+    <row r="32" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="8" t="s">
         <v>107</v>
       </c>
@@ -10520,7 +10544,7 @@
       <c r="DG32" s="12"/>
       <c r="DH32" s="12"/>
     </row>
-    <row r="33" spans="2:112" ht="20" customHeight="1">
+    <row r="33" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="23" t="s">
         <v>107</v>
       </c>
@@ -10773,7 +10797,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="2:112" ht="20" customHeight="1">
+    <row r="34" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="13" t="s">
         <v>107</v>
       </c>
@@ -10917,7 +10941,7 @@
         <v>107</v>
       </c>
       <c r="BD34" s="16" t="s">
-        <v>136</v>
+        <v>285</v>
       </c>
       <c r="BE34" s="16" t="s">
         <v>115</v>
@@ -10983,7 +11007,7 @@
       </c>
       <c r="CS34" s="17"/>
       <c r="CT34" s="16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="CU34" s="16" t="s">
         <v>146</v>
@@ -11001,7 +11025,7 @@
         <v>219</v>
       </c>
       <c r="CZ34" s="16" t="s">
-        <v>219</v>
+        <v>289</v>
       </c>
       <c r="DA34" s="16" t="s">
         <v>149</v>
@@ -11010,547 +11034,991 @@
         <v>271</v>
       </c>
       <c r="DC34" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="DD34" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="DD34" s="16" t="s">
-        <v>271</v>
       </c>
       <c r="DE34" s="16" t="s">
         <v>271</v>
       </c>
       <c r="DF34" s="16" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="DG34" s="16" t="s">
         <v>150</v>
       </c>
       <c r="DH34" s="16" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
     </row>
-    <row r="35" spans="2:112" ht="20" customHeight="1">
-      <c r="B35" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" s="20">
+    <row r="35" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="15">
+        <v>43322421</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1004048015</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="O35" s="16"/>
+      <c r="P35" s="15">
+        <v>19831119</v>
+      </c>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="S35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="T35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="U35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="V35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="W35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="X35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM35" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP35" s="15">
+        <v>20080214</v>
+      </c>
+      <c r="AQ35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR35" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV35" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX35" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ35" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="BA35" s="15">
+        <v>20160214</v>
+      </c>
+      <c r="BB35" s="17"/>
+      <c r="BC35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF35" s="17"/>
+      <c r="BG35" s="17"/>
+      <c r="BH35" s="17"/>
+      <c r="BI35" s="17"/>
+      <c r="BJ35" s="17"/>
+      <c r="BK35" s="17"/>
+      <c r="BL35" s="17"/>
+      <c r="BM35" s="17"/>
+      <c r="BN35" s="17"/>
+      <c r="BO35" s="17"/>
+      <c r="BP35" s="17"/>
+      <c r="BQ35" s="17"/>
+      <c r="BR35" s="17"/>
+      <c r="BS35" s="17"/>
+      <c r="BT35" s="17"/>
+      <c r="BU35" s="17"/>
+      <c r="BV35" s="17"/>
+      <c r="BW35" s="17"/>
+      <c r="BX35" s="17"/>
+      <c r="BY35" s="17"/>
+      <c r="BZ35" s="17"/>
+      <c r="CA35" s="17"/>
+      <c r="CB35" s="17"/>
+      <c r="CC35" s="17"/>
+      <c r="CD35" s="16"/>
+      <c r="CE35" s="17"/>
+      <c r="CF35" s="16"/>
+      <c r="CG35" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH35" s="17"/>
+      <c r="CI35" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="CJ35" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="CK35" s="15">
+        <v>5</v>
+      </c>
+      <c r="CL35" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="CM35" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CN35" s="15">
+        <v>35</v>
+      </c>
+      <c r="CO35" s="17"/>
+      <c r="CP35" s="17"/>
+      <c r="CQ35" s="17"/>
+      <c r="CR35" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS35" s="17"/>
+      <c r="CT35" s="16"/>
+      <c r="CU35" s="16"/>
+      <c r="CV35" s="16"/>
+      <c r="CW35" s="16"/>
+      <c r="CX35" s="16"/>
+      <c r="CY35" s="16"/>
+      <c r="CZ35" s="16"/>
+      <c r="DA35" s="16"/>
+      <c r="DB35" s="16"/>
+      <c r="DC35" s="16"/>
+      <c r="DD35" s="16"/>
+      <c r="DE35" s="16"/>
+      <c r="DF35" s="16"/>
+      <c r="DG35" s="16"/>
+      <c r="DH35" s="16"/>
+    </row>
+    <row r="36" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="15">
+        <v>43322421</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F36" s="15">
+        <v>1004048015</v>
+      </c>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="O36" s="16"/>
+      <c r="P36" s="15">
+        <v>19831119</v>
+      </c>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="S36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="T36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="U36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="V36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="W36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="X36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM36" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP36" s="15">
+        <v>20160214</v>
+      </c>
+      <c r="AQ36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR36" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV36" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AW36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX36" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ36" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="BA36" s="15">
+        <v>20080214</v>
+      </c>
+      <c r="BB36" s="17"/>
+      <c r="BC36" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD36" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="BE36" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF36" s="17"/>
+      <c r="BG36" s="17"/>
+      <c r="BH36" s="17"/>
+      <c r="BI36" s="17"/>
+      <c r="BJ36" s="17"/>
+      <c r="BK36" s="17"/>
+      <c r="BL36" s="17"/>
+      <c r="BM36" s="17"/>
+      <c r="BN36" s="17"/>
+      <c r="BO36" s="17"/>
+      <c r="BP36" s="17"/>
+      <c r="BQ36" s="17"/>
+      <c r="BR36" s="17"/>
+      <c r="BS36" s="17"/>
+      <c r="BT36" s="17"/>
+      <c r="BU36" s="17"/>
+      <c r="BV36" s="17"/>
+      <c r="BW36" s="17"/>
+      <c r="BX36" s="17"/>
+      <c r="BY36" s="17"/>
+      <c r="BZ36" s="17"/>
+      <c r="CA36" s="17"/>
+      <c r="CB36" s="17"/>
+      <c r="CC36" s="17"/>
+      <c r="CD36" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="CE36" s="17"/>
+      <c r="CF36" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="CG36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH36" s="17"/>
+      <c r="CI36" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="CJ36" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="CK36" s="15">
+        <v>5</v>
+      </c>
+      <c r="CL36" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="CM36" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CN36" s="15">
+        <v>35</v>
+      </c>
+      <c r="CO36" s="17"/>
+      <c r="CP36" s="17"/>
+      <c r="CQ36" s="17"/>
+      <c r="CR36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS36" s="17"/>
+      <c r="CT36" s="16"/>
+      <c r="CU36" s="16"/>
+      <c r="CV36" s="16"/>
+      <c r="CW36" s="16"/>
+      <c r="CX36" s="16"/>
+      <c r="CY36" s="16"/>
+      <c r="CZ36" s="16"/>
+      <c r="DA36" s="16"/>
+      <c r="DB36" s="16"/>
+      <c r="DC36" s="16"/>
+      <c r="DD36" s="16"/>
+      <c r="DE36" s="16"/>
+      <c r="DF36" s="16"/>
+      <c r="DG36" s="16"/>
+      <c r="DH36" s="16"/>
+    </row>
+    <row r="37" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="20">
         <v>21345614</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E37" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F35" s="20">
+      <c r="F37" s="20">
         <v>1008743215</v>
       </c>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21" t="s">
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="O35" s="21"/>
-      <c r="P35" s="20">
+      <c r="O37" s="21"/>
+      <c r="P37" s="20">
         <v>19800514</v>
       </c>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="21" t="s">
+      <c r="Q37" s="20"/>
+      <c r="R37" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="S35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="T35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="U35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="V35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="W35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="X35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM35" s="21" t="s">
+      <c r="S37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="U37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="V37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="W37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="X37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM37" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AN35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP35" s="20">
+      <c r="AN37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP37" s="20">
         <v>19940912</v>
       </c>
-      <c r="AQ35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AR35" s="21" t="s">
+      <c r="AQ37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR37" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="AS35" s="21" t="s">
+      <c r="AS37" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="AT35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV35" s="21" t="s">
+      <c r="AT37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV37" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="AW35" s="21" t="s">
+      <c r="AW37" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="AX35" s="21" t="s">
+      <c r="AX37" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AY35" s="21" t="s">
+      <c r="AY37" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="AZ35" s="36" t="s">
+      <c r="AZ37" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="BA35" s="20">
+      <c r="BA37" s="20">
+        <v>19940912</v>
+      </c>
+      <c r="BB37" s="20">
+        <v>222344</v>
+      </c>
+      <c r="BC37" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD37" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="BE37" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF37" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG37" s="22"/>
+      <c r="BH37" s="22"/>
+      <c r="BI37" s="22"/>
+      <c r="BJ37" s="22"/>
+      <c r="BK37" s="22"/>
+      <c r="BL37" s="22"/>
+      <c r="BM37" s="22"/>
+      <c r="BN37" s="22"/>
+      <c r="BO37" s="22"/>
+      <c r="BP37" s="22"/>
+      <c r="BQ37" s="22"/>
+      <c r="BR37" s="22"/>
+      <c r="BS37" s="22"/>
+      <c r="BT37" s="22"/>
+      <c r="BU37" s="22"/>
+      <c r="BV37" s="22"/>
+      <c r="BW37" s="22"/>
+      <c r="BX37" s="22"/>
+      <c r="BY37" s="22"/>
+      <c r="BZ37" s="22"/>
+      <c r="CA37" s="22"/>
+      <c r="CB37" s="22"/>
+      <c r="CC37" s="22"/>
+      <c r="CD37" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="CE37" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="CF37" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="CG37" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH37" s="22"/>
+      <c r="CI37" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="CJ37" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="CK37" s="20">
+        <v>6</v>
+      </c>
+      <c r="CL37" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="CM37" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="CN37" s="20">
+        <v>25</v>
+      </c>
+      <c r="CO37" s="22"/>
+      <c r="CP37" s="22"/>
+      <c r="CQ37" s="22"/>
+      <c r="CR37" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS37" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="CT37" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="CU37" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="CV37" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="CW37" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="CX37" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="CY37" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="CZ37" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="DA37" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DB37" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="DC37" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="DD37" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE37" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="DF37" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="DG37" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="DH37" s="22" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="25">
+        <v>313456</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="26">
+        <v>1008743215</v>
+      </c>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="26"/>
+      <c r="N38" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="O38" s="26"/>
+      <c r="P38" s="25">
+        <v>19820513</v>
+      </c>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="S38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="T38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="U38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="V38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="W38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="X38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM38" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP38" s="25">
+        <v>20120703</v>
+      </c>
+      <c r="AQ38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR38" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS38" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV38" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW38" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX38" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY38" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="AZ38" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA38" s="25">
         <v>20140512</v>
       </c>
-      <c r="BB35" s="20">
+      <c r="BB38" s="25">
         <v>222344</v>
       </c>
-      <c r="BC35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="BD35" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="BE35" s="21" t="s">
+      <c r="BC38" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD38" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="BE38" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="BF35" s="21" t="s">
+      <c r="BF38" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="BG35" s="22"/>
-      <c r="BH35" s="22"/>
-      <c r="BI35" s="22"/>
-      <c r="BJ35" s="22"/>
-      <c r="BK35" s="22"/>
-      <c r="BL35" s="22"/>
-      <c r="BM35" s="22"/>
-      <c r="BN35" s="22"/>
-      <c r="BO35" s="22"/>
-      <c r="BP35" s="22"/>
-      <c r="BQ35" s="22"/>
-      <c r="BR35" s="22"/>
-      <c r="BS35" s="22"/>
-      <c r="BT35" s="22"/>
-      <c r="BU35" s="22"/>
-      <c r="BV35" s="22"/>
-      <c r="BW35" s="22"/>
-      <c r="BX35" s="22"/>
-      <c r="BY35" s="22"/>
-      <c r="BZ35" s="22"/>
-      <c r="CA35" s="22"/>
-      <c r="CB35" s="22"/>
-      <c r="CC35" s="22"/>
-      <c r="CD35" s="21" t="s">
+      <c r="BG38" s="27"/>
+      <c r="BH38" s="27"/>
+      <c r="BI38" s="27"/>
+      <c r="BJ38" s="27"/>
+      <c r="BK38" s="27"/>
+      <c r="BL38" s="27"/>
+      <c r="BM38" s="27"/>
+      <c r="BN38" s="27"/>
+      <c r="BO38" s="27"/>
+      <c r="BP38" s="27"/>
+      <c r="BQ38" s="27"/>
+      <c r="BR38" s="27"/>
+      <c r="BS38" s="27"/>
+      <c r="BT38" s="27"/>
+      <c r="BU38" s="27"/>
+      <c r="BV38" s="27"/>
+      <c r="BW38" s="27"/>
+      <c r="BX38" s="27"/>
+      <c r="BY38" s="27"/>
+      <c r="BZ38" s="27"/>
+      <c r="CA38" s="27"/>
+      <c r="CB38" s="27"/>
+      <c r="CC38" s="27"/>
+      <c r="CD38" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="CE35" s="21" t="s">
+      <c r="CE38" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="CF35" s="21" t="s">
+      <c r="CF38" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="CG35" s="21" t="s">
+      <c r="CG38" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="CH35" s="22"/>
-      <c r="CI35" s="21" t="s">
+      <c r="CH38" s="27"/>
+      <c r="CI38" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="CJ35" s="21" t="s">
+      <c r="CJ38" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="CK35" s="20">
+      <c r="CK38" s="25">
         <v>6</v>
       </c>
-      <c r="CL35" s="21" t="s">
+      <c r="CL38" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="CM35" s="21" t="s">
+      <c r="CM38" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="CN35" s="20">
+      <c r="CN38" s="27">
         <v>25</v>
       </c>
-      <c r="CO35" s="22"/>
-      <c r="CP35" s="22"/>
-      <c r="CQ35" s="22"/>
-      <c r="CR35" s="21" t="s">
+      <c r="CO38" s="27"/>
+      <c r="CP38" s="27"/>
+      <c r="CQ38" s="27"/>
+      <c r="CR38" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="CS35" s="21" t="s">
+      <c r="CS38" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="CT35" s="21" t="s">
+      <c r="CT38" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="CU35" s="21" t="s">
+      <c r="CU38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="CV35" s="21" t="s">
+      <c r="CV38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="CW35" s="21" t="s">
+      <c r="CW38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="CX35" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="CY35" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="CZ35" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="DA35" s="21" t="s">
+      <c r="CX38" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="CY38" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="CZ38" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="DA38" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DB35" s="21" t="s">
+      <c r="DB38" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DC38" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="DC35" s="21" t="s">
+      <c r="DD38" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="DD35" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="DE35" s="21" t="s">
+      <c r="DE38" s="26" t="s">
         <v>271</v>
       </c>
-      <c r="DF35" s="21" t="s">
+      <c r="DF38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG35" s="22" t="s">
+      <c r="DG38" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DH35" s="22" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="36" spans="2:112" ht="20" customHeight="1">
-      <c r="B36" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="25">
-        <v>313456</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="26">
-        <v>1008743215</v>
-      </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="O36" s="26"/>
-      <c r="P36" s="25">
-        <v>19820513</v>
-      </c>
-      <c r="Q36" s="25"/>
-      <c r="R36" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="S36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="T36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="U36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="V36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="W36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="X36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AD36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AE36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AL36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM36" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AO36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP36" s="25">
-        <v>20120703</v>
-      </c>
-      <c r="AQ36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AR36" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS36" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="AT36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="AV36" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="AW36" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="AX36" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="AY36" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="AZ36" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="BA36" s="25">
-        <v>20140512</v>
-      </c>
-      <c r="BB36" s="25">
-        <v>222344</v>
-      </c>
-      <c r="BC36" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="BD36" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="BE36" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="BF36" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="BG36" s="27"/>
-      <c r="BH36" s="27"/>
-      <c r="BI36" s="27"/>
-      <c r="BJ36" s="27"/>
-      <c r="BK36" s="27"/>
-      <c r="BL36" s="27"/>
-      <c r="BM36" s="27"/>
-      <c r="BN36" s="27"/>
-      <c r="BO36" s="27"/>
-      <c r="BP36" s="27"/>
-      <c r="BQ36" s="27"/>
-      <c r="BR36" s="27"/>
-      <c r="BS36" s="27"/>
-      <c r="BT36" s="27"/>
-      <c r="BU36" s="27"/>
-      <c r="BV36" s="27"/>
-      <c r="BW36" s="27"/>
-      <c r="BX36" s="27"/>
-      <c r="BY36" s="27"/>
-      <c r="BZ36" s="27"/>
-      <c r="CA36" s="27"/>
-      <c r="CB36" s="27"/>
-      <c r="CC36" s="27"/>
-      <c r="CD36" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="CE36" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="CF36" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="CG36" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="CH36" s="27"/>
-      <c r="CI36" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="CJ36" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="CK36" s="25">
-        <v>6</v>
-      </c>
-      <c r="CL36" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="CM36" s="26" t="s">
-        <v>178</v>
-      </c>
-      <c r="CN36" s="27">
-        <v>25</v>
-      </c>
-      <c r="CO36" s="27"/>
-      <c r="CP36" s="27"/>
-      <c r="CQ36" s="27"/>
-      <c r="CR36" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="CS36" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="CT36" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="CU36" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="CV36" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="CW36" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="CX36" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="CY36" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="CZ36" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="DA36" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="DB36" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="DC36" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="DD36" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="DE36" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="DF36" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="DG36" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="DH36" s="26" t="s">
+      <c r="DH38" s="26" t="s">
         <v>283</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove Los Angeles eligibility flow
- Move convictions file output tests to use configurable eligibility
- Eliminate LA specific tests

[#164714845]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newuser/go/src/gogen/test_fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D094EB-54BE-5E4C-9813-1BAF24E11A00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -900,7 +894,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1120,8 +1114,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1472,7 +1490,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1509,6 +1527,10 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1545,6 +1567,10 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2699,118 +2725,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:DH38"/>
+  <dimension ref="A1:DH38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CT1" workbookViewId="0">
-      <selection activeCell="DA48" sqref="DA48"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="BD46" sqref="BD46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.33203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" customWidth="1"/>
-    <col min="19" max="20" width="8" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="12.83203125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="18" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="1" customWidth="1"/>
-    <col min="29" max="29" width="7.83203125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="8.1640625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5" style="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5" style="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="10.83203125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1640625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="16.5" style="1" customWidth="1"/>
-    <col min="37" max="37" width="13.5" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.83203125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="10.1640625" style="1" customWidth="1"/>
-    <col min="40" max="40" width="13" style="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5" style="1" customWidth="1"/>
-    <col min="42" max="42" width="16.1640625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5" style="1" customWidth="1"/>
-    <col min="44" max="44" width="21.6640625" style="1" customWidth="1"/>
-    <col min="45" max="45" width="13.6640625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="20.33203125" style="1" customWidth="1"/>
-    <col min="47" max="47" width="14.1640625" style="1" customWidth="1"/>
-    <col min="48" max="48" width="19.5" style="1" customWidth="1"/>
-    <col min="49" max="50" width="19.6640625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="13.33203125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="12.6640625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5" style="1" customWidth="1"/>
-    <col min="54" max="54" width="7" style="1" customWidth="1"/>
-    <col min="55" max="55" width="14.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="12" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="8" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="1" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="7.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5" style="1" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5" style="1" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="11.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="10.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5" style="1" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5" style="1" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="21.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="46" max="46" width="20.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5" style="1" hidden="1" customWidth="1"/>
+    <col min="49" max="50" width="19.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="7" style="1" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="14.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="13.6640625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" style="1" customWidth="1"/>
-    <col min="59" max="59" width="19.6640625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="20.6640625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" style="1" customWidth="1"/>
-    <col min="62" max="62" width="23.33203125" style="1" customWidth="1"/>
-    <col min="63" max="63" width="21.6640625" style="1" customWidth="1"/>
-    <col min="64" max="64" width="20.5" style="1" customWidth="1"/>
-    <col min="65" max="65" width="21.5" style="1" customWidth="1"/>
-    <col min="66" max="66" width="19.33203125" style="1" customWidth="1"/>
-    <col min="67" max="67" width="24.33203125" style="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1640625" style="1" customWidth="1"/>
-    <col min="69" max="69" width="17.1640625" style="1" customWidth="1"/>
-    <col min="70" max="70" width="20" style="1" customWidth="1"/>
-    <col min="71" max="71" width="13" style="1" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="1" customWidth="1"/>
-    <col min="73" max="74" width="17.1640625" style="1" customWidth="1"/>
-    <col min="75" max="77" width="16.6640625" style="1" customWidth="1"/>
-    <col min="78" max="78" width="18" style="1" customWidth="1"/>
-    <col min="79" max="79" width="17.6640625" style="1" customWidth="1"/>
-    <col min="80" max="80" width="12.1640625" style="1" customWidth="1"/>
-    <col min="81" max="81" width="11" style="1" customWidth="1"/>
-    <col min="82" max="82" width="26.33203125" style="1" customWidth="1"/>
-    <col min="83" max="83" width="16.83203125" style="1" customWidth="1"/>
-    <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
-    <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
-    <col min="87" max="87" width="16" style="1" customWidth="1"/>
-    <col min="88" max="88" width="16.83203125" style="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" style="1" customWidth="1"/>
-    <col min="90" max="90" width="16.5" style="1" customWidth="1"/>
-    <col min="91" max="91" width="17.33203125" style="1" customWidth="1"/>
-    <col min="92" max="92" width="9.33203125" style="1" customWidth="1"/>
-    <col min="93" max="93" width="8.83203125" style="1" customWidth="1"/>
-    <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
-    <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
-    <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
-    <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
-    <col min="98" max="98" width="24" style="1" customWidth="1"/>
-    <col min="99" max="101" width="23.6640625" style="1" customWidth="1"/>
-    <col min="102" max="102" width="12.5" style="1" customWidth="1"/>
-    <col min="103" max="103" width="23.5" style="1" customWidth="1"/>
-    <col min="104" max="104" width="23.1640625" style="1" customWidth="1"/>
-    <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
-    <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
+    <col min="57" max="57" width="13.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="18.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="19.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="18.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="23.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="20.5" style="1" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="21.5" style="1" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="19.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="24.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="15.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="69" max="69" width="17.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="20" style="1" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="13" style="1" hidden="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="73" max="74" width="17.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="75" max="77" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="18" style="1" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="17.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="12.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="81" max="81" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="26.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="16.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="84" max="84" width="17.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="85" max="85" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="87" max="87" width="16" style="1" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="16.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="13.5" style="1" hidden="1" customWidth="1"/>
+    <col min="90" max="90" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="92" max="92" width="9.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="93" max="93" width="8.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="94" max="94" width="15.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="95" max="95" width="26.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="96" max="96" width="12.5" style="1" hidden="1" customWidth="1"/>
+    <col min="97" max="97" width="29.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="98" max="98" width="24" style="1" hidden="1" customWidth="1"/>
+    <col min="99" max="101" width="23.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="102" max="102" width="12.5" style="1" hidden="1" customWidth="1"/>
+    <col min="103" max="103" width="23.5" style="1" hidden="1" customWidth="1"/>
+    <col min="104" max="104" width="23.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="105" max="109" width="20.5" style="1" hidden="1" customWidth="1"/>
+    <col min="110" max="110" width="25.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="111" max="111" width="25.83203125" style="1" customWidth="1"/>
     <col min="112" max="112" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:112" s="42" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:112" s="42" customFormat="1" ht="27.75" customHeight="1">
       <c r="B1" s="39" t="s">
         <v>253</v>
       </c>
@@ -2997,7 +3024,10 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="2:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:112" ht="20.25" customHeight="1">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3332,7 +3362,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:112" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:112" ht="20.25" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
@@ -3553,7 +3583,7 @@
       <c r="DG3" s="7"/>
       <c r="DH3" s="7"/>
     </row>
-    <row r="4" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:112" ht="20" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
@@ -3784,7 +3814,7 @@
       <c r="DG4" s="12"/>
       <c r="DH4" s="12"/>
     </row>
-    <row r="5" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:112" ht="20" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>107</v>
       </c>
@@ -4005,7 +4035,7 @@
       <c r="DG5" s="12"/>
       <c r="DH5" s="12"/>
     </row>
-    <row r="6" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:112" ht="20" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4226,7 +4256,7 @@
       <c r="DG6" s="12"/>
       <c r="DH6" s="12"/>
     </row>
-    <row r="7" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:112" ht="20" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>107</v>
       </c>
@@ -4447,7 +4477,10 @@
       <c r="DG7" s="12"/>
       <c r="DH7" s="12"/>
     </row>
-    <row r="8" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:112" ht="20" customHeight="1">
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
       <c r="B8" s="8" t="s">
         <v>107</v>
       </c>
@@ -4710,7 +4743,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:112" ht="20" customHeight="1">
       <c r="B9" s="23" t="s">
         <v>107</v>
       </c>
@@ -4931,7 +4964,10 @@
       <c r="DG9" s="26"/>
       <c r="DH9" s="26"/>
     </row>
-    <row r="10" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:112" ht="20" customHeight="1">
+      <c r="A10" t="b">
+        <v>1</v>
+      </c>
       <c r="B10" s="23" t="s">
         <v>107</v>
       </c>
@@ -5194,7 +5230,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:112" ht="20" customHeight="1">
       <c r="B11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5411,7 +5447,10 @@
       <c r="DG11" s="26"/>
       <c r="DH11" s="26"/>
     </row>
-    <row r="12" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:112" ht="20" customHeight="1">
+      <c r="A12" t="b">
+        <v>1</v>
+      </c>
       <c r="B12" s="23" t="s">
         <v>107</v>
       </c>
@@ -5674,7 +5713,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:112" ht="20" customHeight="1">
       <c r="B13" s="23" t="s">
         <v>107</v>
       </c>
@@ -5899,7 +5938,10 @@
       <c r="DG13" s="26"/>
       <c r="DH13" s="26"/>
     </row>
-    <row r="14" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:112" ht="20" customHeight="1">
+      <c r="A14" t="b">
+        <v>1</v>
+      </c>
       <c r="B14" s="13" t="s">
         <v>107</v>
       </c>
@@ -6164,7 +6206,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:112" ht="20" customHeight="1">
       <c r="B15" s="13" t="s">
         <v>107</v>
       </c>
@@ -6395,7 +6437,7 @@
       <c r="DG15" s="17"/>
       <c r="DH15" s="17"/>
     </row>
-    <row r="16" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:112" ht="20" customHeight="1">
       <c r="B16" s="13" t="s">
         <v>107</v>
       </c>
@@ -6626,7 +6668,10 @@
       <c r="DG16" s="17"/>
       <c r="DH16" s="17"/>
     </row>
-    <row r="17" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:112" ht="20" customHeight="1">
+      <c r="A17" t="b">
+        <v>1</v>
+      </c>
       <c r="B17" s="13" t="s">
         <v>107</v>
       </c>
@@ -6889,7 +6934,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:112" ht="20" customHeight="1">
       <c r="B18" s="13" t="s">
         <v>107</v>
       </c>
@@ -7118,7 +7163,7 @@
       <c r="DG18" s="17"/>
       <c r="DH18" s="17"/>
     </row>
-    <row r="19" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:112" ht="20" customHeight="1">
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
@@ -7349,7 +7394,10 @@
       <c r="DG19" s="22"/>
       <c r="DH19" s="22"/>
     </row>
-    <row r="20" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:112" ht="20" customHeight="1">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
       <c r="B20" s="18" t="s">
         <v>181</v>
       </c>
@@ -7606,7 +7654,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="21" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:112" ht="20" customHeight="1">
       <c r="B21" s="18" t="s">
         <v>107</v>
       </c>
@@ -7837,7 +7885,10 @@
       <c r="DG21" s="22"/>
       <c r="DH21" s="22"/>
     </row>
-    <row r="22" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:112" ht="20" customHeight="1">
+      <c r="A22" t="b">
+        <v>1</v>
+      </c>
       <c r="B22" s="18" t="s">
         <v>107</v>
       </c>
@@ -8100,7 +8151,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:112" ht="20" customHeight="1">
+      <c r="A23" t="b">
+        <v>1</v>
+      </c>
       <c r="B23" s="23" t="s">
         <v>107</v>
       </c>
@@ -8359,7 +8413,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:112" ht="20" customHeight="1">
       <c r="B24" s="23" t="s">
         <v>107</v>
       </c>
@@ -8586,7 +8640,7 @@
       <c r="DG24" s="27"/>
       <c r="DH24" s="27"/>
     </row>
-    <row r="25" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:112" ht="20" customHeight="1">
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -8799,7 +8853,10 @@
       <c r="DG25" s="27"/>
       <c r="DH25" s="27"/>
     </row>
-    <row r="26" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:112" ht="20" customHeight="1">
+      <c r="A26" t="b">
+        <v>1</v>
+      </c>
       <c r="B26" s="23" t="s">
         <v>107</v>
       </c>
@@ -9046,7 +9103,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:112" ht="20" customHeight="1">
+      <c r="A27" t="b">
+        <v>1</v>
+      </c>
       <c r="B27" s="23" t="s">
         <v>107</v>
       </c>
@@ -9293,7 +9353,10 @@
         <v>278</v>
       </c>
     </row>
-    <row r="28" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:112" ht="20" customHeight="1">
+      <c r="A28" t="b">
+        <v>1</v>
+      </c>
       <c r="B28" s="28" t="s">
         <v>107</v>
       </c>
@@ -9556,7 +9619,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="29" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:112" ht="20" customHeight="1">
       <c r="B29" s="28" t="s">
         <v>107</v>
       </c>
@@ -9787,7 +9850,10 @@
       <c r="DG29" s="32"/>
       <c r="DH29" s="32"/>
     </row>
-    <row r="30" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:112" ht="20" customHeight="1">
+      <c r="A30" t="b">
+        <v>1</v>
+      </c>
       <c r="B30" s="28" t="s">
         <v>107</v>
       </c>
@@ -10050,7 +10116,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:112" ht="20" customHeight="1">
+      <c r="A31" t="b">
+        <v>1</v>
+      </c>
       <c r="B31" s="8" t="s">
         <v>107</v>
       </c>
@@ -10313,7 +10382,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="32" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:112" ht="20" customHeight="1">
       <c r="B32" s="8" t="s">
         <v>107</v>
       </c>
@@ -10544,7 +10613,10 @@
       <c r="DG32" s="12"/>
       <c r="DH32" s="12"/>
     </row>
-    <row r="33" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:112" ht="20" customHeight="1">
+      <c r="A33" t="b">
+        <v>1</v>
+      </c>
       <c r="B33" s="23" t="s">
         <v>107</v>
       </c>
@@ -10797,7 +10869,10 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:112" ht="20" customHeight="1">
+      <c r="A34" t="b">
+        <v>1</v>
+      </c>
       <c r="B34" s="13" t="s">
         <v>107</v>
       </c>
@@ -11052,7 +11127,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:112" ht="20" customHeight="1">
       <c r="B35" s="13" t="s">
         <v>107</v>
       </c>
@@ -11271,7 +11346,7 @@
       <c r="DG35" s="16"/>
       <c r="DH35" s="16"/>
     </row>
-    <row r="36" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:112" ht="20" customHeight="1">
       <c r="B36" s="13" t="s">
         <v>107</v>
       </c>
@@ -11496,7 +11571,10 @@
       <c r="DG36" s="16"/>
       <c r="DH36" s="16"/>
     </row>
-    <row r="37" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:112" ht="20" customHeight="1">
+      <c r="A37" t="b">
+        <v>1</v>
+      </c>
       <c r="B37" s="18" t="s">
         <v>107</v>
       </c>
@@ -11759,7 +11837,10 @@
         <v>263</v>
       </c>
     </row>
-    <row r="38" spans="2:112" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:112" ht="20" customHeight="1">
+      <c r="A38" t="b">
+        <v>1</v>
+      </c>
       <c r="B38" s="23" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Count individuals who will get some type of relief
Added fixture in configurable_flow.xlsx where an individual gets no
relief.

[#167770422]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27340"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="291">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>3.7</t>
+  </si>
+  <si>
+    <t>BLOFELD,ERNST</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1117,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1490,7 +1511,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1531,6 +1552,9 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1571,6 +1595,9 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2729,111 +2756,112 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DH38"/>
+  <dimension ref="A1:DH39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BD46" sqref="BD46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
+      <pane ySplit="1200" topLeftCell="A11" activePane="bottomLeft"/>
+      <selection activeCell="AT1" sqref="AT1"/>
+      <selection pane="bottomLeft" activeCell="DH39" sqref="DH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="13" width="12" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="8" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="12.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="18.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="18" style="1" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="1" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="7.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="8.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="15.5" style="1" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5" style="1" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="10.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="11.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="10.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5" style="1" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="16.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5" style="1" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="21.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="13.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="20.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="14.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="19.5" style="1" hidden="1" customWidth="1"/>
-    <col min="49" max="50" width="19.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="13.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="10.5" style="1" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="7" style="1" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="14.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.33203125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" customWidth="1"/>
+    <col min="19" max="20" width="8" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="18.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="18" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="1" customWidth="1"/>
+    <col min="29" max="29" width="7.83203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.5" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5" style="1" customWidth="1"/>
+    <col min="33" max="33" width="10.6640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.83203125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="16.5" style="1" customWidth="1"/>
+    <col min="37" max="37" width="13.5" style="1" customWidth="1"/>
+    <col min="38" max="38" width="11.83203125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="10.1640625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="13" style="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5" style="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5" style="1" customWidth="1"/>
+    <col min="44" max="44" width="21.6640625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="13.6640625" style="1" customWidth="1"/>
+    <col min="46" max="46" width="20.33203125" style="1" customWidth="1"/>
+    <col min="47" max="47" width="14.1640625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5" style="1" customWidth="1"/>
+    <col min="49" max="50" width="19.6640625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="13.33203125" style="1" customWidth="1"/>
+    <col min="52" max="52" width="12.6640625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="10.5" style="1" customWidth="1"/>
+    <col min="54" max="54" width="7" style="1" customWidth="1"/>
+    <col min="55" max="55" width="14.83203125" style="1" customWidth="1"/>
     <col min="56" max="56" width="37.6640625" style="1" customWidth="1"/>
-    <col min="57" max="57" width="13.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="18.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="19.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="20.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="23.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="21.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="20.5" style="1" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="21.5" style="1" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="19.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="24.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="69" max="69" width="17.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="20" style="1" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="13" style="1" hidden="1" customWidth="1"/>
-    <col min="72" max="72" width="16.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="73" max="74" width="17.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="75" max="77" width="16.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="78" max="78" width="18" style="1" hidden="1" customWidth="1"/>
-    <col min="79" max="79" width="17.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="12.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="81" max="81" width="11" style="1" hidden="1" customWidth="1"/>
-    <col min="82" max="82" width="26.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="83" max="83" width="16.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="84" max="84" width="17.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="85" max="85" width="14.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="87" max="87" width="16" style="1" hidden="1" customWidth="1"/>
-    <col min="88" max="88" width="16.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" style="1" hidden="1" customWidth="1"/>
-    <col min="90" max="90" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="17.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="92" max="92" width="9.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="93" max="93" width="8.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="94" max="94" width="15.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="95" max="95" width="26.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="96" max="96" width="12.5" style="1" hidden="1" customWidth="1"/>
-    <col min="97" max="97" width="29.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="98" max="98" width="24" style="1" hidden="1" customWidth="1"/>
-    <col min="99" max="101" width="23.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="102" max="102" width="12.5" style="1" hidden="1" customWidth="1"/>
-    <col min="103" max="103" width="23.5" style="1" hidden="1" customWidth="1"/>
-    <col min="104" max="104" width="23.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="105" max="109" width="20.5" style="1" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="25.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="111" max="111" width="25.83203125" style="1" customWidth="1"/>
+    <col min="57" max="57" width="13.6640625" style="1" customWidth="1"/>
+    <col min="58" max="58" width="18.6640625" style="1" customWidth="1"/>
+    <col min="59" max="59" width="19.6640625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="20.6640625" style="1" customWidth="1"/>
+    <col min="61" max="61" width="18.33203125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="23.33203125" style="1" customWidth="1"/>
+    <col min="63" max="63" width="21.6640625" style="1" customWidth="1"/>
+    <col min="64" max="64" width="20.5" style="1" customWidth="1"/>
+    <col min="65" max="65" width="21.5" style="1" customWidth="1"/>
+    <col min="66" max="66" width="19.33203125" style="1" customWidth="1"/>
+    <col min="67" max="67" width="24.33203125" style="1" customWidth="1"/>
+    <col min="68" max="68" width="15.1640625" style="1" customWidth="1"/>
+    <col min="69" max="69" width="17.1640625" style="1" customWidth="1"/>
+    <col min="70" max="70" width="20" style="1" customWidth="1"/>
+    <col min="71" max="71" width="13" style="1" customWidth="1"/>
+    <col min="72" max="72" width="16.33203125" style="1" customWidth="1"/>
+    <col min="73" max="74" width="17.1640625" style="1" customWidth="1"/>
+    <col min="75" max="77" width="16.6640625" style="1" customWidth="1"/>
+    <col min="78" max="78" width="18" style="1" customWidth="1"/>
+    <col min="79" max="79" width="17.6640625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="12.1640625" style="1" customWidth="1"/>
+    <col min="81" max="81" width="11" style="1" customWidth="1"/>
+    <col min="82" max="82" width="26.33203125" style="1" customWidth="1"/>
+    <col min="83" max="83" width="16.83203125" style="1" customWidth="1"/>
+    <col min="84" max="84" width="17.6640625" style="1" customWidth="1"/>
+    <col min="85" max="85" width="14.33203125" style="1" customWidth="1"/>
+    <col min="86" max="86" width="12.6640625" style="1" customWidth="1"/>
+    <col min="87" max="87" width="16" style="1" customWidth="1"/>
+    <col min="88" max="88" width="16.83203125" style="1" customWidth="1"/>
+    <col min="89" max="89" width="13.5" style="1" customWidth="1"/>
+    <col min="90" max="90" width="16.5" style="1" customWidth="1"/>
+    <col min="91" max="91" width="17.33203125" style="1" customWidth="1"/>
+    <col min="92" max="92" width="9.33203125" style="1" customWidth="1"/>
+    <col min="93" max="93" width="8.83203125" style="1" customWidth="1"/>
+    <col min="94" max="94" width="15.33203125" style="1" customWidth="1"/>
+    <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
+    <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
+    <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
+    <col min="98" max="98" width="24" style="1" customWidth="1"/>
+    <col min="99" max="101" width="23.6640625" style="1" customWidth="1"/>
+    <col min="102" max="102" width="12.5" style="1" customWidth="1"/>
+    <col min="103" max="103" width="23.5" style="1" customWidth="1"/>
+    <col min="104" max="104" width="23.1640625" style="1" customWidth="1"/>
+    <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
+    <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
     <col min="112" max="112" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12103,6 +12131,235 @@
         <v>283</v>
       </c>
     </row>
+    <row r="39" spans="1:112" ht="20" customHeight="1">
+      <c r="B39" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="30">
+        <v>313457</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" s="30">
+        <v>1008743218</v>
+      </c>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="30"/>
+      <c r="N39" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="O39" s="31"/>
+      <c r="P39" s="30">
+        <v>19700305</v>
+      </c>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="S39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="T39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="U39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="V39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="W39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="X39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM39" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP39" s="30">
+        <v>20120703</v>
+      </c>
+      <c r="AQ39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR39" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS39" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV39" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW39" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX39" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY39" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="AZ39" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA39" s="30">
+        <v>20140512</v>
+      </c>
+      <c r="BB39" s="30"/>
+      <c r="BC39" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD39" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE39" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF39" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG39" s="32"/>
+      <c r="BH39" s="32"/>
+      <c r="BI39" s="32"/>
+      <c r="BJ39" s="32"/>
+      <c r="BK39" s="32"/>
+      <c r="BL39" s="32"/>
+      <c r="BM39" s="32"/>
+      <c r="BN39" s="32"/>
+      <c r="BO39" s="32"/>
+      <c r="BP39" s="32"/>
+      <c r="BQ39" s="32"/>
+      <c r="BR39" s="32"/>
+      <c r="BS39" s="32"/>
+      <c r="BT39" s="32"/>
+      <c r="BU39" s="32"/>
+      <c r="BV39" s="32"/>
+      <c r="BW39" s="32"/>
+      <c r="BX39" s="32"/>
+      <c r="BY39" s="32"/>
+      <c r="BZ39" s="32"/>
+      <c r="CA39" s="32"/>
+      <c r="CB39" s="32"/>
+      <c r="CC39" s="32"/>
+      <c r="CD39" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="CE39" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="CF39" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="CG39" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH39" s="32"/>
+      <c r="CI39" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="CJ39" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="CK39" s="30">
+        <v>6</v>
+      </c>
+      <c r="CL39" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="CM39" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="CN39" s="30">
+        <v>25</v>
+      </c>
+      <c r="CO39" s="32"/>
+      <c r="CP39" s="32"/>
+      <c r="CQ39" s="32"/>
+      <c r="CR39" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS39" s="31"/>
+      <c r="CT39" s="31"/>
+      <c r="CU39" s="31"/>
+      <c r="CV39" s="31"/>
+      <c r="CW39" s="31"/>
+      <c r="CX39" s="31"/>
+      <c r="CY39" s="31"/>
+      <c r="CZ39" s="31"/>
+      <c r="DA39" s="31"/>
+      <c r="DB39" s="31"/>
+      <c r="DC39" s="31"/>
+      <c r="DD39" s="31"/>
+      <c r="DE39" s="31"/>
+      <c r="DF39" s="31"/>
+      <c r="DG39" s="31"/>
+      <c r="DH39" s="31"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Consolidate HS 11357 subsections into a single HS 11357
[#16771735]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="289">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -783,9 +783,6 @@
     <t>hello</t>
   </si>
   <si>
-    <t>11357(B)HS-POSSESS MARIJUANA</t>
-  </si>
-  <si>
     <t>PALPATINE,SHEEV</t>
   </si>
   <si>
@@ -852,9 +849,6 @@
     <t>Dismiss all HS 11358 convictions</t>
   </si>
   <si>
-    <t>Dismiss all HS 11357(c) convictions</t>
-  </si>
-  <si>
     <t>Reduce all HS 11359 convictions</t>
   </si>
   <si>
@@ -870,9 +864,6 @@
     <t>7.4</t>
   </si>
   <si>
-    <t>Dismiss all HS 11357 convictions (when no sub-section is specified)</t>
-  </si>
-  <si>
     <t>Individual is deceased</t>
   </si>
   <si>
@@ -892,6 +883,9 @@
   </si>
   <si>
     <t>BLOFELD,ERNST</t>
+  </si>
+  <si>
+    <t>Dismiss all HS 11357 convictions</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1111,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1511,7 +1511,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1555,6 +1555,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1598,6 +1599,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2758,10 +2760,10 @@
   </sheetPr>
   <dimension ref="A1:DH39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
-      <pane ySplit="1200" topLeftCell="A11" activePane="bottomLeft"/>
-      <selection activeCell="AT1" sqref="AT1"/>
-      <selection pane="bottomLeft" activeCell="DH39" sqref="DH39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CR1" workbookViewId="0">
+      <pane ySplit="1200" activePane="bottomLeft"/>
+      <selection activeCell="BB1" sqref="BB1"/>
+      <selection pane="bottomLeft" activeCell="CZ17" sqref="CZ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3369,16 +3371,16 @@
         <v>103</v>
       </c>
       <c r="DB2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="DC2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="DE2" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="DF2" s="2" t="s">
         <v>104</v>
@@ -4750,16 +4752,16 @@
         <v>149</v>
       </c>
       <c r="DB8" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC8" s="11" t="s">
         <v>149</v>
       </c>
       <c r="DD8" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DE8" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF8" s="11" t="s">
         <v>104</v>
@@ -4768,7 +4770,7 @@
         <v>150</v>
       </c>
       <c r="DH8" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:112" ht="20" customHeight="1">
@@ -5231,22 +5233,22 @@
         <v>159</v>
       </c>
       <c r="CZ10" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="DA10" s="26" t="s">
         <v>145</v>
       </c>
       <c r="DB10" s="26" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="DC10" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD10" s="26" t="s">
-        <v>271</v>
+        <v>149</v>
       </c>
       <c r="DE10" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF10" s="26" t="s">
         <v>146</v>
@@ -5255,7 +5257,7 @@
         <v>150</v>
       </c>
       <c r="DH10" s="26" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:112" ht="20" customHeight="1">
@@ -5624,7 +5626,7 @@
         <v>107</v>
       </c>
       <c r="BD12" s="26" t="s">
-        <v>254</v>
+        <v>174</v>
       </c>
       <c r="BE12" s="26" t="s">
         <v>115</v>
@@ -5708,28 +5710,28 @@
         <v>157</v>
       </c>
       <c r="CX12" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="CY12" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="CZ12" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="DA12" s="26" t="s">
         <v>145</v>
       </c>
       <c r="DB12" s="26" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="DC12" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD12" s="26" t="s">
-        <v>271</v>
+        <v>149</v>
       </c>
       <c r="DE12" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF12" s="26" t="s">
         <v>146</v>
@@ -5738,7 +5740,7 @@
         <v>150</v>
       </c>
       <c r="DH12" s="26" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:112" ht="20" customHeight="1">
@@ -6207,13 +6209,13 @@
         <v>148</v>
       </c>
       <c r="CZ14" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="DA14" s="16" t="s">
         <v>169</v>
       </c>
       <c r="DB14" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC14" s="16" t="s">
         <v>156</v>
@@ -6222,7 +6224,7 @@
         <v>149</v>
       </c>
       <c r="DE14" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF14" s="16" t="s">
         <v>146</v>
@@ -6231,7 +6233,7 @@
         <v>150</v>
       </c>
       <c r="DH14" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:112" ht="20" customHeight="1">
@@ -6929,19 +6931,19 @@
         <v>146</v>
       </c>
       <c r="CX17" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="CY17" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="CZ17" s="16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="DA17" s="16" t="s">
         <v>169</v>
       </c>
       <c r="DB17" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC17" s="16" t="s">
         <v>156</v>
@@ -6950,7 +6952,7 @@
         <v>149</v>
       </c>
       <c r="DE17" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF17" s="16" t="s">
         <v>146</v>
@@ -6959,7 +6961,7 @@
         <v>150</v>
       </c>
       <c r="DH17" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:112" ht="20" customHeight="1">
@@ -7649,19 +7651,19 @@
         <v>146</v>
       </c>
       <c r="CX20" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="CY20" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="CY20" s="21" t="s">
-        <v>268</v>
-      </c>
       <c r="CZ20" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="DA20" s="21" t="s">
         <v>145</v>
       </c>
       <c r="DB20" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC20" s="21" t="s">
         <v>149</v>
@@ -7670,7 +7672,7 @@
         <v>149</v>
       </c>
       <c r="DE20" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF20" s="21" t="s">
         <v>146</v>
@@ -7679,7 +7681,7 @@
         <v>150</v>
       </c>
       <c r="DH20" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:112" ht="20" customHeight="1">
@@ -8146,19 +8148,19 @@
         <v>146</v>
       </c>
       <c r="CX22" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="CY22" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="CY22" s="21" t="s">
-        <v>268</v>
-      </c>
       <c r="CZ22" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="DA22" s="21" t="s">
         <v>145</v>
       </c>
       <c r="DB22" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC22" s="21" t="s">
         <v>149</v>
@@ -8167,7 +8169,7 @@
         <v>149</v>
       </c>
       <c r="DE22" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF22" s="21" t="s">
         <v>146</v>
@@ -8429,7 +8431,7 @@
         <v>149</v>
       </c>
       <c r="DE23" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF23" s="26" t="s">
         <v>146</v>
@@ -8438,7 +8440,7 @@
         <v>150</v>
       </c>
       <c r="DH23" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:112" ht="20" customHeight="1">
@@ -9119,7 +9121,7 @@
         <v>149</v>
       </c>
       <c r="DE26" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF26" s="26" t="s">
         <v>146</v>
@@ -9369,7 +9371,7 @@
         <v>149</v>
       </c>
       <c r="DE27" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF27" s="26" t="s">
         <v>146</v>
@@ -9378,7 +9380,7 @@
         <v>184</v>
       </c>
       <c r="DH27" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:112" ht="20" customHeight="1">
@@ -9614,10 +9616,10 @@
         <v>146</v>
       </c>
       <c r="CX28" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="CY28" s="31" t="s">
         <v>265</v>
-      </c>
-      <c r="CY28" s="31" t="s">
-        <v>266</v>
       </c>
       <c r="CZ28" s="31" t="s">
         <v>206</v>
@@ -9626,16 +9628,16 @@
         <v>156</v>
       </c>
       <c r="DB28" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC28" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD28" s="31" t="s">
         <v>156</v>
       </c>
       <c r="DE28" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF28" s="31" t="s">
         <v>146</v>
@@ -9644,7 +9646,7 @@
         <v>150</v>
       </c>
       <c r="DH28" s="31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:112" ht="20" customHeight="1">
@@ -10123,16 +10125,16 @@
         <v>156</v>
       </c>
       <c r="DB30" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC30" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD30" s="31" t="s">
         <v>156</v>
       </c>
       <c r="DE30" s="31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF30" s="31" t="s">
         <v>146</v>
@@ -10389,16 +10391,16 @@
         <v>149</v>
       </c>
       <c r="DB31" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC31" s="11" t="s">
         <v>149</v>
       </c>
       <c r="DD31" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DE31" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF31" s="11" t="s">
         <v>146</v>
@@ -10407,7 +10409,7 @@
         <v>150</v>
       </c>
       <c r="DH31" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:112" ht="20" customHeight="1">
@@ -10876,16 +10878,16 @@
         <v>149</v>
       </c>
       <c r="DB33" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC33" s="26" t="s">
         <v>149</v>
       </c>
       <c r="DD33" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DE33" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF33" s="26" t="s">
         <v>146</v>
@@ -10894,7 +10896,7 @@
         <v>150</v>
       </c>
       <c r="DH33" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:112" ht="20" customHeight="1">
@@ -11044,7 +11046,7 @@
         <v>107</v>
       </c>
       <c r="BD34" s="16" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="BE34" s="16" t="s">
         <v>115</v>
@@ -11128,22 +11130,22 @@
         <v>219</v>
       </c>
       <c r="CZ34" s="16" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="DA34" s="16" t="s">
         <v>149</v>
       </c>
       <c r="DB34" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC34" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD34" s="16" t="s">
         <v>149</v>
       </c>
       <c r="DE34" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF34" s="16" t="s">
         <v>104</v>
@@ -11152,7 +11154,7 @@
         <v>150</v>
       </c>
       <c r="DH34" s="16" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:112" ht="20" customHeight="1">
@@ -11289,7 +11291,7 @@
         <v>107</v>
       </c>
       <c r="AZ35" s="35" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="BA35" s="15">
         <v>20160214</v>
@@ -11508,7 +11510,7 @@
         <v>107</v>
       </c>
       <c r="AZ36" s="35" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="BA36" s="15">
         <v>20080214</v>
@@ -11518,7 +11520,7 @@
         <v>107</v>
       </c>
       <c r="BD36" s="16" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="BE36" s="16" t="s">
         <v>115</v>
@@ -11626,7 +11628,7 @@
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
       <c r="N37" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O37" s="21"/>
       <c r="P37" s="20">
@@ -11817,7 +11819,7 @@
         <v>108</v>
       </c>
       <c r="CS37" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="CT37" s="21" t="s">
         <v>149</v>
@@ -11832,28 +11834,28 @@
         <v>146</v>
       </c>
       <c r="CX37" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="CY37" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="CY37" s="21" t="s">
-        <v>262</v>
-      </c>
       <c r="CZ37" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="DA37" s="21" t="s">
         <v>149</v>
       </c>
       <c r="DB37" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DC37" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD37" s="21" t="s">
         <v>149</v>
       </c>
       <c r="DE37" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF37" s="21" t="s">
         <v>146</v>
@@ -11862,7 +11864,7 @@
         <v>150</v>
       </c>
       <c r="DH37" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:112" ht="20" customHeight="1">
@@ -11892,7 +11894,7 @@
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="26" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O38" s="26"/>
       <c r="P38" s="25">
@@ -12014,7 +12016,7 @@
         <v>107</v>
       </c>
       <c r="BD38" s="26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="BE38" s="26" t="s">
         <v>131</v>
@@ -12083,7 +12085,7 @@
         <v>108</v>
       </c>
       <c r="CS38" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="CT38" s="26" t="s">
         <v>149</v>
@@ -12098,13 +12100,13 @@
         <v>146</v>
       </c>
       <c r="CX38" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="CY38" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="CZ38" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="DA38" s="26" t="s">
         <v>149</v>
@@ -12113,13 +12115,13 @@
         <v>149</v>
       </c>
       <c r="DC38" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DD38" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DE38" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="DF38" s="26" t="s">
         <v>146</v>
@@ -12128,7 +12130,7 @@
         <v>150</v>
       </c>
       <c r="DH38" s="26" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:112" ht="20" customHeight="1">
@@ -12155,7 +12157,7 @@
       <c r="L39" s="31"/>
       <c r="M39" s="30"/>
       <c r="N39" s="31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="O39" s="31"/>
       <c r="P39" s="30">

</xml_diff>